<commit_message>
Update lookups and uncertainties file
</commit_message>
<xml_diff>
--- a/2_ModelAndParameters/uncertainties.xlsx
+++ b/2_ModelAndParameters/uncertainties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77C9AF1-7B5B-4532-AC5D-04A8BD05C3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82815870-B5D4-4628-B657-9C229279A0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12377" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="uncertain parameters" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="85">
   <si>
     <t>Unit</t>
   </si>
@@ -315,6 +315,12 @@
   </si>
   <si>
     <t>This sheet defines the uncertain parameters and converts them into formats for ema-workbench</t>
+  </si>
+  <si>
+    <t>CHANGE IN BIKE PARKING PER ADDED SPACE FOR CYCLISTS</t>
+  </si>
+  <si>
+    <t>It is uncertain to what extent bike parking availability will be expanded compared to the current number of bike parking spots per ha of space for cyclists. This uncertainty ranges between zero expansion, and doubling bike parking spots per added space for cyclists.</t>
   </si>
 </sst>
 </file>
@@ -488,19 +494,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -522,6 +519,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,13 +556,13 @@
       <sheetName val="callibration"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
       <sheetData sheetId="7">
         <row r="40">
           <cell r="D40">
@@ -849,10 +849,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0809C193-648C-4CF0-8724-48F7ACFFC1FA}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A2:L92"/>
+  <dimension ref="A2:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -871,7 +871,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="31.3" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>81</v>
       </c>
     </row>
@@ -881,60 +881,60 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="23" t="s">
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="20" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="20"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" s="8" t="s">
+      <c r="I7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="K7" s="19"/>
+      <c r="K7" s="16"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8">
@@ -952,13 +952,13 @@
       <c r="E8" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="15">
         <v>0.5</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="14">
         <v>2</v>
       </c>
-      <c r="H8" s="17"/>
+      <c r="H8" s="14"/>
       <c r="I8" t="s">
         <v>32</v>
       </c>
@@ -968,7 +968,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9">
-        <f>A8+1</f>
+        <f t="shared" ref="A9:A30" si="0">A8+1</f>
         <v>2</v>
       </c>
       <c r="B9" t="s">
@@ -983,14 +983,14 @@
       <c r="E9" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="12">
         <v>0.58399999999999996</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="12">
         <f>F9+(0.018*3)</f>
         <v>0.6379999999999999</v>
       </c>
-      <c r="H9" s="11"/>
+      <c r="H9" s="8"/>
       <c r="I9" t="s">
         <v>32</v>
       </c>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10">
-        <f>A9+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B10" t="s">
@@ -1015,13 +1015,13 @@
       <c r="E10" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="16">
-        <v>0</v>
-      </c>
-      <c r="G10" s="15">
+      <c r="F10" s="13">
+        <v>0</v>
+      </c>
+      <c r="G10" s="12">
         <v>0.28999999999999998</v>
       </c>
-      <c r="H10" s="11"/>
+      <c r="H10" s="8"/>
       <c r="I10" t="s">
         <v>32</v>
       </c>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11">
-        <f>A10+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B11" t="s">
@@ -1046,13 +1046,13 @@
       <c r="E11" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="13">
-        <v>0</v>
-      </c>
-      <c r="G11" s="13">
+      <c r="F11" s="10">
+        <v>0</v>
+      </c>
+      <c r="G11" s="10">
         <v>0.3</v>
       </c>
-      <c r="H11" s="11"/>
+      <c r="H11" s="8"/>
       <c r="I11" t="s">
         <v>69</v>
       </c>
@@ -1062,38 +1062,38 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12">
-        <f>A11+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="G12" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="H12" s="14"/>
+        <v>83</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0</v>
+      </c>
+      <c r="G12" s="10">
+        <v>2</v>
+      </c>
+      <c r="H12" s="8"/>
       <c r="I12" t="s">
         <v>32</v>
       </c>
       <c r="J12" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13">
-        <f>A12+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B13" t="s">
@@ -1103,61 +1103,59 @@
         <v>52</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="G13" s="14">
-        <v>2</v>
-      </c>
-      <c r="H13" s="14"/>
+        <v>67</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="G13" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="H13" s="11"/>
       <c r="I13" t="s">
         <v>32</v>
       </c>
       <c r="J13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14">
-        <f>A13+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
         <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="14">
-        <v>0</v>
-      </c>
-      <c r="G14" s="14">
-        <v>1</v>
-      </c>
-      <c r="H14" s="14">
-        <v>1</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="11">
+        <v>2</v>
+      </c>
+      <c r="H14" s="11"/>
       <c r="I14" t="s">
         <v>32</v>
       </c>
       <c r="J14" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15">
-        <f>A14+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B15" t="s">
@@ -1167,28 +1165,30 @@
         <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="G15" s="14">
-        <v>2</v>
-      </c>
-      <c r="H15" s="14"/>
+        <v>62</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0</v>
+      </c>
+      <c r="G15" s="11">
+        <v>1</v>
+      </c>
+      <c r="H15" s="11">
+        <v>1</v>
+      </c>
       <c r="I15" t="s">
         <v>32</v>
       </c>
       <c r="J15" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16">
-        <f>A15+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B16" t="s">
@@ -1201,15 +1201,15 @@
         <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="14">
+        <v>60</v>
+      </c>
+      <c r="F16" s="11">
         <v>0.5</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="11">
         <v>2</v>
       </c>
-      <c r="H16" s="14"/>
+      <c r="H16" s="11"/>
       <c r="I16" t="s">
         <v>32</v>
       </c>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17">
-        <f>A16+1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B17" t="s">
@@ -1229,28 +1229,28 @@
         <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="14">
-        <v>1</v>
-      </c>
-      <c r="G17" s="14">
-        <v>3</v>
-      </c>
-      <c r="H17" s="14"/>
+        <v>59</v>
+      </c>
+      <c r="F17" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="11">
+        <v>2</v>
+      </c>
+      <c r="H17" s="11"/>
       <c r="I17" t="s">
         <v>32</v>
       </c>
       <c r="J17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18">
-        <f>A17+1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B18" t="s">
@@ -1263,25 +1263,25 @@
         <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="G18" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="H18" s="14"/>
+        <v>57</v>
+      </c>
+      <c r="F18" s="11">
+        <v>1</v>
+      </c>
+      <c r="G18" s="11">
+        <v>3</v>
+      </c>
+      <c r="H18" s="11"/>
       <c r="I18" t="s">
         <v>32</v>
       </c>
       <c r="J18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19">
-        <f>A18+1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B19" t="s">
@@ -1291,56 +1291,56 @@
         <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="14">
-        <v>0</v>
-      </c>
-      <c r="G19" s="14">
-        <v>1</v>
-      </c>
-      <c r="H19" s="14">
-        <v>1</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="F19" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="G19" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="H19" s="11"/>
       <c r="I19" t="s">
         <v>32</v>
       </c>
       <c r="J19" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20">
-        <f>A19+1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="G20" s="14">
-        <v>2</v>
-      </c>
-      <c r="H20" s="14"/>
+        <v>50</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0</v>
+      </c>
+      <c r="G20" s="11">
+        <v>1</v>
+      </c>
+      <c r="H20" s="11">
+        <v>1</v>
+      </c>
       <c r="I20" t="s">
         <v>32</v>
       </c>
       <c r="J20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.4">
@@ -1358,25 +1358,25 @@
         <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" s="14">
+        <v>48</v>
+      </c>
+      <c r="F21" s="11">
         <v>0.5</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="11">
         <v>2</v>
       </c>
-      <c r="H21" s="14"/>
+      <c r="H21" s="11"/>
       <c r="I21" t="s">
         <v>32</v>
       </c>
       <c r="J21" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22">
-        <f>A21+1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B22" t="s">
@@ -1389,25 +1389,25 @@
         <v>34</v>
       </c>
       <c r="E22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="14">
+        <v>46</v>
+      </c>
+      <c r="F22" s="11">
         <v>0.5</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="11">
         <v>2</v>
       </c>
-      <c r="H22" s="14"/>
+      <c r="H22" s="11"/>
       <c r="I22" t="s">
         <v>32</v>
       </c>
       <c r="J22" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23">
-        <f>A22+1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B23" t="s">
@@ -1420,25 +1420,25 @@
         <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="14">
+        <v>44</v>
+      </c>
+      <c r="F23" s="11">
         <v>0.5</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="11">
         <v>2</v>
       </c>
-      <c r="H23" s="14"/>
+      <c r="H23" s="11"/>
       <c r="I23" t="s">
         <v>32</v>
       </c>
       <c r="J23" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24">
-        <f>A23+1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B24" t="s">
@@ -1448,59 +1448,59 @@
         <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="14">
-        <v>1</v>
-      </c>
-      <c r="G24" s="14">
-        <v>5</v>
-      </c>
-      <c r="H24" s="14"/>
+        <v>42</v>
+      </c>
+      <c r="F24" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="11">
+        <v>2</v>
+      </c>
+      <c r="H24" s="11"/>
       <c r="I24" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="J24" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25">
-        <f>A24+1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B25" t="s">
         <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="13">
-        <v>0.5</v>
+        <v>40</v>
+      </c>
+      <c r="F25" s="11">
+        <v>1</v>
       </c>
       <c r="G25" s="11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H25" s="11"/>
       <c r="I25" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J25" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26">
-        <f>A25+1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B26" t="s">
@@ -1513,235 +1513,245 @@
         <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="13">
+        <v>37</v>
+      </c>
+      <c r="F26" s="10">
         <v>0.5</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="8">
         <v>2</v>
       </c>
-      <c r="H26" s="11"/>
+      <c r="H26" s="8"/>
       <c r="I26" t="s">
         <v>32</v>
       </c>
       <c r="J26" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27">
-        <f>A26+1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E27" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" s="12">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="G27" s="12">
-        <v>1.5E-3</v>
-      </c>
-      <c r="H27" s="11"/>
+        <v>33</v>
+      </c>
+      <c r="F27" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="8">
+        <v>2</v>
+      </c>
+      <c r="H27" s="8"/>
       <c r="I27" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="J27" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28">
-        <f>A27+1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D28" t="s">
         <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="G28" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="H28" s="11"/>
+        <v>28</v>
+      </c>
+      <c r="F28" s="9">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G28" s="9">
+        <v>1.5E-3</v>
+      </c>
+      <c r="H28" s="8"/>
       <c r="I28" t="s">
         <v>20</v>
       </c>
       <c r="J28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="G29" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="H29" s="8"/>
+      <c r="I29" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29">
-        <f>A28+1</f>
+    <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E29" s="8" t="s">
+      <c r="E30" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F30" s="7">
         <v>1E-3</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G30" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H29" s="9"/>
-      <c r="I29" s="8" t="s">
+      <c r="H30" s="6"/>
+      <c r="I30" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="8" t="s">
+      <c r="J30" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B34" s="24" t="s">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B35" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="F34" s="24" t="s">
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="F35" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B35" t="s">
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B36" t="s">
         <v>11</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>10</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>9</v>
       </c>
-      <c r="F35" t="str" cm="1">
-        <f t="array" ref="F35">"['"&amp;_xlfn.TEXTJOIN("', '",TRUE,_xlfn._xlws.FILTER(E8:E29,$D$8:$D$29="effect sensitivity"))&amp;"']"</f>
+      <c r="F36" t="str" cm="1">
+        <f t="array" ref="F36">"['"&amp;_xlfn.TEXTJOIN("', '",TRUE,_xlfn._xlws.FILTER(E8:E30,$D$8:$D$30="effect sensitivity"))&amp;"']"</f>
         <v>['RENEWAL RATE SENSITIVITY', 'CAR ADOPTION SENSITIVITY TO USAGE', 'BIKE ADOPTION SENSITIVITY TO PARKING', 'BIKE ADOPTION SENSITIVITY TO USAGE', 'CAR NETWORK DISTANCE SENSITIVITY', 'CYCLING NETWORK DISTANCE SENSITIVITY', 'SUBJECTIVE CYCLING TIME SENSITIVITY', 'PARKING SEARCH AND EGRESS SENSITIVITY', 'SENSITIVITY TO SIDEWALK DATA UNCERTAINTY', 'SENSITIVITY TO CAR LANE DATA UNCERTAINTY']</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B36" t="str" cm="1">
-        <f t="array" ref="B36:B45">_xlfn._xlws.FILTER(E8:E29,$D$8:$D$29="constant")</f>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B37" t="str" cm="1">
+        <f t="array" ref="B37:B47">_xlfn._xlws.FILTER(E8:E30,$D$8:$D$30="constant")</f>
         <v>DESIRED PEDESTRIAN SPACE SHARE</v>
       </c>
-      <c r="C36" cm="1">
-        <f t="array" ref="C36:C45">_xlfn._xlws.FILTER(F8:F29,$D$8:$D$29="constant")</f>
+      <c r="C37" cm="1">
+        <f t="array" ref="C37:C47">_xlfn._xlws.FILTER(F8:F30,$D$8:$D$30="constant")</f>
         <v>0.58399999999999996</v>
       </c>
-      <c r="D36" cm="1">
-        <f t="array" ref="D36:D45">_xlfn._xlws.FILTER(G8:G29,$D$8:$D$29="constant")</f>
+      <c r="D37" cm="1">
+        <f t="array" ref="D37:D47">_xlfn._xlws.FILTER(G8:G30,$D$8:$D$30="constant")</f>
         <v>0.6379999999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B37" t="str">
-        <v>DESIRED SHARE OF CAR SPACE USED FOR PARKING</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="J37" t="s">
-        <v>18</v>
-      </c>
-      <c r="K37">
-        <v>10</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B38" t="str">
-        <v>PARKING SPOTS PER HOME CONSTRUCTED</v>
+        <v>DESIRED SHARE OF CAR SPACE USED FOR PARKING</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>0.3</v>
-      </c>
-      <c r="K38" t="s">
-        <v>17</v>
-      </c>
-      <c r="L38" t="s">
-        <v>16</v>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="J38" t="s">
+        <v>18</v>
+      </c>
+      <c r="K38">
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B39" t="str">
-        <v>REFERENCE SHIFT IN CAR ADOPTION</v>
+        <v>PARKING SPOTS PER HOME CONSTRUCTED</v>
       </c>
       <c r="C39">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="D39">
-        <v>0.25</v>
-      </c>
-      <c r="J39" t="s">
-        <v>15</v>
-      </c>
-      <c r="K39">
-        <v>0.01</v>
-      </c>
-      <c r="L39" s="7">
-        <f>1-(1-K39)^(1/$K$37)</f>
-        <v>1.0045287082499632E-3</v>
+        <v>0.3</v>
+      </c>
+      <c r="K39" t="s">
+        <v>17</v>
+      </c>
+      <c r="L39" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B40" t="str">
-        <v>CONTACT RATE</v>
+        <v>CHANGE IN BIKE PARKING PER ADDED SPACE FOR CYCLISTS</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J40" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K40">
-        <v>0.03</v>
-      </c>
-      <c r="L40" s="7">
-        <f>1-(1-K40)^(1/$K$37)</f>
-        <v>3.0412866381062109E-3</v>
+        <v>0.01</v>
+      </c>
+      <c r="L40" s="4">
+        <f>1-(1-K40)^(1/$K$38)</f>
+        <v>1.0045287082499632E-3</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B41" t="str">
-        <v>BIKESHARING TO PRIVATE BIKE UPGRADE FRACTION</v>
+        <v>REFERENCE SHIFT IN CAR ADOPTION</v>
       </c>
       <c r="C41">
         <v>0.05</v>
@@ -1750,1144 +1760,1224 @@
         <v>0.25</v>
       </c>
       <c r="J41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K41">
-        <v>0.05</v>
-      </c>
-      <c r="L41" s="7">
-        <f>1-(1-K41)^(1/$K$37)</f>
-        <v>5.1161968918237433E-3</v>
+        <v>0.03</v>
+      </c>
+      <c r="L41" s="4">
+        <f>1-(1-K41)^(1/$K$38)</f>
+        <v>3.0412866381062109E-3</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B42" t="str">
-        <v>PERCEPTION TIME</v>
+        <v>CONTACT RATE</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="J42" t="s">
+        <v>13</v>
+      </c>
+      <c r="K42">
+        <v>0.05</v>
+      </c>
+      <c r="L42" s="4">
+        <f>1-(1-K42)^(1/$K$38)</f>
+        <v>5.1161968918237433E-3</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B43" t="str">
-        <v>NET ADDED PT CAPACITY PER YEAR</v>
+        <v>BIKESHARING TO PRIVATE BIKE UPGRADE FRACTION</v>
       </c>
       <c r="C43">
-        <v>5.0000000000000001E-4</v>
+        <v>0.05</v>
       </c>
       <c r="D43">
-        <v>1.5E-3</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B44" t="str">
-        <v>DESTINATION SHIFT RATE RING</v>
+        <v>PERCEPTION TIME</v>
       </c>
       <c r="C44">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="D44">
-        <v>0.01</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B45" t="str">
+        <v>NET ADDED PT CAPACITY PER YEAR</v>
+      </c>
+      <c r="C45">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D45">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B46" t="str">
+        <v>DESTINATION SHIFT RATE RING</v>
+      </c>
+      <c r="C46">
+        <v>1E-3</v>
+      </c>
+      <c r="D46">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B47" t="str">
         <v>DESTINATION SHIFT RATE CITY</v>
       </c>
-      <c r="C45">
+      <c r="C47">
         <v>1E-3</v>
       </c>
-      <c r="D45">
+      <c r="D47">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="48" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="6" t="s">
+    <row r="49" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B49" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C49" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D49" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="E49" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="F49" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G48" s="6" t="s">
+      <c r="G49" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H48" s="6" t="s">
+      <c r="H49" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I48" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B49" s="2" t="str" cm="1">
-        <f t="array" ref="B49">INDEX($B$8:$I$30,INT((ROW(B49)-49)/2)+1,COLUMN(B49)-1)</f>
+      <c r="I49" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B50" s="1" t="str" cm="1">
+        <f t="array" ref="B50">INDEX($B$8:$I$31,INT((ROW(B50)-49)/2)+1,COLUMN(B50)-1)</f>
         <v>Public space</v>
       </c>
-      <c r="C49" s="2" t="str" cm="1">
-        <f t="array" ref="C49">INDEX($B$8:$I$30,INT((ROW(C49)-49)/2)+1,COLUMN(C49)-1)</f>
+      <c r="C50" s="1" t="str" cm="1">
+        <f t="array" ref="C50">INDEX($B$8:$I$31,INT((ROW(C50)-49)/2)+1,COLUMN(C50)-1)</f>
         <v>Future policy</v>
       </c>
-      <c r="D49" s="2" t="str" cm="1">
-        <f t="array" ref="D49">INDEX($B$8:$I$30,INT((ROW(D49)-49)/2)+1,COLUMN(D49)-1)</f>
+      <c r="D50" s="1" t="str" cm="1">
+        <f t="array" ref="D50">INDEX($B$8:$I$31,INT((ROW(D50)-49)/2)+1,COLUMN(D50)-1)</f>
         <v>effect sensitivity</v>
       </c>
-      <c r="E49" s="2" t="str" cm="1">
-        <f t="array" ref="E49">INDEX($B$8:$I$30,INT((ROW(E49)-49)/2)+1,COLUMN(E49)-1)</f>
+      <c r="E50" s="1" t="str" cm="1">
+        <f t="array" ref="E50">INDEX($B$8:$I$31,INT((ROW(E50)-49)/2)+1,COLUMN(E50)-1)</f>
         <v>RENEWAL RATE SENSITIVITY</v>
       </c>
-      <c r="F49" s="2" cm="1">
-        <f t="array" ref="F49">INDEX($B$8:$I$30,INT((ROW(F49)-49)/2)+1,COLUMN(F49)-1)</f>
+      <c r="F50" s="1" cm="1">
+        <f t="array" ref="F50">INDEX($B$8:$I$31,INT((ROW(F50)-49)/2)+1,COLUMN(F50)-1)</f>
         <v>0.5</v>
       </c>
-      <c r="G49" s="2" cm="1">
-        <f t="array" ref="G49">INDEX($B$8:$I$30,INT((ROW(G49)-49)/2)+1,COLUMN(G49)-1)</f>
+      <c r="G50" s="1" cm="1">
+        <f t="array" ref="G50">INDEX($B$8:$I$31,INT((ROW(G50)-49)/2)+1,COLUMN(G50)-1)</f>
         <v>2</v>
       </c>
-      <c r="H49" s="2" cm="1">
-        <f t="array" ref="H49">INDEX($B$8:$I$30,INT((ROW(H49)-49)/2)+1,COLUMN(H49)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I49" s="2" t="str" cm="1">
-        <f t="array" ref="I49">INDEX($B$8:$I$30,INT((ROW(I49)-49)/2)+1,COLUMN(I49)-1)</f>
+      <c r="H50" s="1" cm="1">
+        <f t="array" ref="H50">INDEX($B$8:$I$31,INT((ROW(H50)-49)/2)+1,COLUMN(H50)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I50" s="1" t="str" cm="1">
+        <f t="array" ref="I50">INDEX($B$8:$I$31,INT((ROW(I50)-49)/2)+1,COLUMN(I50)-1)</f>
         <v>Dmnl</v>
       </c>
     </row>
-    <row r="50" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="3" t="str" cm="1">
-        <f t="array" ref="B50">IF(MOD(ROW(B50)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B50)-49)/2)+1),"")</f>
+    <row r="51" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B51" s="24" t="str" cm="1">
+        <f t="array" ref="B51">IF(MOD(ROW(B50)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B50)-49)/2)+1),"")</f>
         <v>The base assumption is for the renewal rate to increase by one third of its current value by the time cycling uptake reaches 50% of the population (see Appendix ). Since this effect size is uncertain, it is varied by X^y if X is the normalized effect from the base assumption, and y varies between 0.5 and 2.</v>
       </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B51" s="2" t="str" cm="1">
-        <f t="array" ref="B51">INDEX($B$8:$I$30,INT((ROW(B51)-49)/2)+1,COLUMN(B51)-1)</f>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="24"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B52" s="1" t="str" cm="1">
+        <f t="array" ref="B52">INDEX($B$8:$I$31,INT((ROW(B52)-49)/2)+1,COLUMN(B52)-1)</f>
         <v>Public space</v>
       </c>
-      <c r="C51" s="2" t="str" cm="1">
-        <f t="array" ref="C51">INDEX($B$8:$I$30,INT((ROW(C51)-49)/2)+1,COLUMN(C51)-1)</f>
+      <c r="C52" s="1" t="str" cm="1">
+        <f t="array" ref="C52">INDEX($B$8:$I$31,INT((ROW(C52)-49)/2)+1,COLUMN(C52)-1)</f>
         <v>Future policy</v>
       </c>
-      <c r="D51" s="2" t="str" cm="1">
-        <f t="array" ref="D51">INDEX($B$8:$I$30,INT((ROW(D51)-49)/2)+1,COLUMN(D51)-1)</f>
+      <c r="D52" s="1" t="str" cm="1">
+        <f t="array" ref="D52">INDEX($B$8:$I$31,INT((ROW(D52)-49)/2)+1,COLUMN(D52)-1)</f>
         <v>constant</v>
       </c>
-      <c r="E51" s="2" t="str" cm="1">
-        <f t="array" ref="E51">INDEX($B$8:$I$30,INT((ROW(E51)-49)/2)+1,COLUMN(E51)-1)</f>
+      <c r="E52" s="1" t="str" cm="1">
+        <f t="array" ref="E52">INDEX($B$8:$I$31,INT((ROW(E52)-49)/2)+1,COLUMN(E52)-1)</f>
         <v>DESIRED PEDESTRIAN SPACE SHARE</v>
       </c>
-      <c r="F51" s="2" cm="1">
-        <f t="array" ref="F51">INDEX($B$8:$I$30,INT((ROW(F51)-49)/2)+1,COLUMN(F51)-1)</f>
+      <c r="F52" s="1" cm="1">
+        <f t="array" ref="F52">INDEX($B$8:$I$31,INT((ROW(F52)-49)/2)+1,COLUMN(F52)-1)</f>
         <v>0.58399999999999996</v>
       </c>
-      <c r="G51" s="2" cm="1">
-        <f t="array" ref="G51">INDEX($B$8:$I$30,INT((ROW(G51)-49)/2)+1,COLUMN(G51)-1)</f>
+      <c r="G52" s="1" cm="1">
+        <f t="array" ref="G52">INDEX($B$8:$I$31,INT((ROW(G52)-49)/2)+1,COLUMN(G52)-1)</f>
         <v>0.6379999999999999</v>
       </c>
-      <c r="H51" s="2" cm="1">
-        <f t="array" ref="H51">INDEX($B$8:$I$30,INT((ROW(H51)-49)/2)+1,COLUMN(H51)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I51" s="2" t="str" cm="1">
-        <f t="array" ref="I51">INDEX($B$8:$I$30,INT((ROW(I51)-49)/2)+1,COLUMN(I51)-1)</f>
+      <c r="H52" s="1" cm="1">
+        <f t="array" ref="H52">INDEX($B$8:$I$31,INT((ROW(H52)-49)/2)+1,COLUMN(H52)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I52" s="1" t="str" cm="1">
+        <f t="array" ref="I52">INDEX($B$8:$I$31,INT((ROW(I52)-49)/2)+1,COLUMN(I52)-1)</f>
         <v>Dmnl</v>
       </c>
     </row>
-    <row r="52" spans="2:9" ht="45.45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="5" t="str" cm="1">
-        <f t="array" ref="B52">IF(MOD(ROW(B52)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B52)-49)/2)+1),"")</f>
+    <row r="53" spans="2:9" ht="45.45" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B53" s="24" t="str" cm="1">
+        <f t="array" ref="B53">IF(MOD(ROW(B52)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B52)-49)/2)+1),"")</f>
         <v>Pedestrian space share would increase by 1.8%-points (to 58.4% based on estimate for current share) on average if the full road network was reallocated in proportion to current reallocation plans. Since the final ambition for pedestrianization is uncertain and may increase, this share is varied between a 1.8% and 7.2%-point increase (four times current ambition).</v>
       </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B53" s="2" t="str" cm="1">
-        <f t="array" ref="B53">INDEX($B$8:$I$30,INT((ROW(B53)-49)/2)+1,COLUMN(B53)-1)</f>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
+      <c r="H53" s="24"/>
+      <c r="I53" s="24"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B54" s="1" t="str" cm="1">
+        <f t="array" ref="B54">INDEX($B$8:$I$31,INT((ROW(B54)-49)/2)+1,COLUMN(B54)-1)</f>
         <v>Public space</v>
       </c>
-      <c r="C53" s="2" t="str" cm="1">
-        <f t="array" ref="C53">INDEX($B$8:$I$30,INT((ROW(C53)-49)/2)+1,COLUMN(C53)-1)</f>
+      <c r="C54" s="1" t="str" cm="1">
+        <f t="array" ref="C54">INDEX($B$8:$I$31,INT((ROW(C54)-49)/2)+1,COLUMN(C54)-1)</f>
         <v>Future policy</v>
       </c>
-      <c r="D53" s="2" t="str" cm="1">
-        <f t="array" ref="D53">INDEX($B$8:$I$30,INT((ROW(D53)-49)/2)+1,COLUMN(D53)-1)</f>
+      <c r="D54" s="1" t="str" cm="1">
+        <f t="array" ref="D54">INDEX($B$8:$I$31,INT((ROW(D54)-49)/2)+1,COLUMN(D54)-1)</f>
         <v>constant</v>
       </c>
-      <c r="E53" s="2" t="str" cm="1">
-        <f t="array" ref="E53">INDEX($B$8:$I$30,INT((ROW(E53)-49)/2)+1,COLUMN(E53)-1)</f>
+      <c r="E54" s="1" t="str" cm="1">
+        <f t="array" ref="E54">INDEX($B$8:$I$31,INT((ROW(E54)-49)/2)+1,COLUMN(E54)-1)</f>
         <v>DESIRED SHARE OF CAR SPACE USED FOR PARKING</v>
       </c>
-      <c r="F53" s="2" cm="1">
-        <f t="array" ref="F53">INDEX($B$8:$I$30,INT((ROW(F53)-49)/2)+1,COLUMN(F53)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="G53" s="2" cm="1">
-        <f t="array" ref="G53">INDEX($B$8:$I$30,INT((ROW(G53)-49)/2)+1,COLUMN(G53)-1)</f>
+      <c r="F54" s="1" cm="1">
+        <f t="array" ref="F54">INDEX($B$8:$I$31,INT((ROW(F54)-49)/2)+1,COLUMN(F54)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="G54" s="1" cm="1">
+        <f t="array" ref="G54">INDEX($B$8:$I$31,INT((ROW(G54)-49)/2)+1,COLUMN(G54)-1)</f>
         <v>0.28999999999999998</v>
       </c>
-      <c r="H53" s="2" cm="1">
-        <f t="array" ref="H53">INDEX($B$8:$I$30,INT((ROW(H53)-49)/2)+1,COLUMN(H53)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I53" s="2" t="str" cm="1">
-        <f t="array" ref="I53">INDEX($B$8:$I$30,INT((ROW(I53)-49)/2)+1,COLUMN(I53)-1)</f>
+      <c r="H54" s="1" cm="1">
+        <f t="array" ref="H54">INDEX($B$8:$I$31,INT((ROW(H54)-49)/2)+1,COLUMN(H54)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I54" s="1" t="str" cm="1">
+        <f t="array" ref="I54">INDEX($B$8:$I$31,INT((ROW(I54)-49)/2)+1,COLUMN(I54)-1)</f>
         <v>Dmnl</v>
       </c>
     </row>
-    <row r="54" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B54" s="3" t="str" cm="1">
-        <f t="array" ref="B54">IF(MOD(ROW(B54)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B54)-49)/2)+1),"")</f>
+    <row r="55" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B55" s="24" t="str" cm="1">
+        <f t="array" ref="B55">IF(MOD(ROW(B54)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B54)-49)/2)+1),"")</f>
         <v>Currently, 19% of space for motorists is parking space. This is uncertain: road space reallocation could consume parking space to a larger or smaller extent. The desired share is varied between zero on-street parking and 10%-points more than today.</v>
       </c>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B55" s="4" t="str" cm="1">
-        <f t="array" ref="B55">INDEX($B$8:$I$30,INT((ROW(B55)-49)/2)+1,COLUMN(B55)-1)</f>
+      <c r="C55" s="24"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="24"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B56" s="2" t="str" cm="1">
+        <f t="array" ref="B56">INDEX($B$8:$I$31,INT((ROW(B56)-49)/2)+1,COLUMN(B56)-1)</f>
         <v>Public space</v>
       </c>
-      <c r="C55" s="4" t="str" cm="1">
-        <f t="array" ref="C55">INDEX($B$8:$I$30,INT((ROW(C55)-49)/2)+1,COLUMN(C55)-1)</f>
+      <c r="C56" s="2" t="str" cm="1">
+        <f t="array" ref="C56">INDEX($B$8:$I$31,INT((ROW(C56)-49)/2)+1,COLUMN(C56)-1)</f>
         <v>Future policy</v>
       </c>
-      <c r="D55" s="4" t="str" cm="1">
-        <f t="array" ref="D55">INDEX($B$8:$I$30,INT((ROW(D55)-49)/2)+1,COLUMN(D55)-1)</f>
+      <c r="D56" s="2" t="str" cm="1">
+        <f t="array" ref="D56">INDEX($B$8:$I$31,INT((ROW(D56)-49)/2)+1,COLUMN(D56)-1)</f>
         <v>constant</v>
       </c>
-      <c r="E55" s="4" t="str" cm="1">
-        <f t="array" ref="E55">INDEX($B$8:$I$30,INT((ROW(E55)-49)/2)+1,COLUMN(E55)-1)</f>
+      <c r="E56" s="2" t="str" cm="1">
+        <f t="array" ref="E56">INDEX($B$8:$I$31,INT((ROW(E56)-49)/2)+1,COLUMN(E56)-1)</f>
         <v>PARKING SPOTS PER HOME CONSTRUCTED</v>
       </c>
-      <c r="F55" s="4" cm="1">
-        <f t="array" ref="F55">INDEX($B$8:$I$30,INT((ROW(F55)-49)/2)+1,COLUMN(F55)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="G55" s="4" cm="1">
-        <f t="array" ref="G55">INDEX($B$8:$I$30,INT((ROW(G55)-49)/2)+1,COLUMN(G55)-1)</f>
+      <c r="F56" s="2" cm="1">
+        <f t="array" ref="F56">INDEX($B$8:$I$31,INT((ROW(F56)-49)/2)+1,COLUMN(F56)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="G56" s="2" cm="1">
+        <f t="array" ref="G56">INDEX($B$8:$I$31,INT((ROW(G56)-49)/2)+1,COLUMN(G56)-1)</f>
         <v>0.3</v>
       </c>
-      <c r="H55" s="4" cm="1">
-        <f t="array" ref="H55">INDEX($B$8:$I$30,INT((ROW(H55)-49)/2)+1,COLUMN(H55)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I55" s="4" t="str" cm="1">
-        <f t="array" ref="I55">INDEX($B$8:$I$30,INT((ROW(I55)-49)/2)+1,COLUMN(I55)-1)</f>
+      <c r="H56" s="2" cm="1">
+        <f t="array" ref="H56">INDEX($B$8:$I$31,INT((ROW(H56)-49)/2)+1,COLUMN(H56)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I56" s="2" t="str" cm="1">
+        <f t="array" ref="I56">INDEX($B$8:$I$31,INT((ROW(I56)-49)/2)+1,COLUMN(I56)-1)</f>
         <v>spots/homes</v>
       </c>
     </row>
-    <row r="56" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B56" s="3" t="str" cm="1">
-        <f t="array" ref="B56">IF(MOD(ROW(B56)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B56)-49)/2)+1),"")</f>
+    <row r="57" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B57" s="24" t="str" cm="1">
+        <f t="array" ref="B57">IF(MOD(ROW(B56)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B56)-49)/2)+1),"")</f>
         <v>Currently, there are 0.33 residential parking spots per home in the city. This is expected to decline in future residential housing, but to which extent is uncertain. The chosen range is between 0 and 0.3 parking spots per home</v>
       </c>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B57" s="2" t="str" cm="1">
-        <f t="array" ref="B57">INDEX($B$8:$I$30,INT((ROW(B57)-49)/2)+1,COLUMN(B57)-1)</f>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="24"/>
+      <c r="H57" s="24"/>
+      <c r="I57" s="24"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B58" s="1" t="str" cm="1">
+        <f t="array" ref="B58">INDEX($B$8:$I$31,INT((ROW(B58)-49)/2)+1,COLUMN(B58)-1)</f>
+        <v>Public space</v>
+      </c>
+      <c r="C58" s="1" t="str" cm="1">
+        <f t="array" ref="C58">INDEX($B$8:$I$31,INT((ROW(C58)-49)/2)+1,COLUMN(C58)-1)</f>
+        <v>Future policy</v>
+      </c>
+      <c r="D58" s="1" t="str" cm="1">
+        <f t="array" ref="D58">INDEX($B$8:$I$31,INT((ROW(D58)-49)/2)+1,COLUMN(D58)-1)</f>
+        <v>constant</v>
+      </c>
+      <c r="E58" s="1" t="str" cm="1">
+        <f t="array" ref="E58">INDEX($B$8:$I$31,INT((ROW(E58)-49)/2)+1,COLUMN(E58)-1)</f>
+        <v>CHANGE IN BIKE PARKING PER ADDED SPACE FOR CYCLISTS</v>
+      </c>
+      <c r="F58" s="1" cm="1">
+        <f t="array" ref="F58">INDEX($B$8:$I$31,INT((ROW(F58)-49)/2)+1,COLUMN(F58)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="G58" s="1" cm="1">
+        <f t="array" ref="G58">INDEX($B$8:$I$31,INT((ROW(G58)-49)/2)+1,COLUMN(G58)-1)</f>
+        <v>2</v>
+      </c>
+      <c r="H58" s="1" cm="1">
+        <f t="array" ref="H58">INDEX($B$8:$I$31,INT((ROW(H58)-49)/2)+1,COLUMN(H58)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I58" s="1" t="str" cm="1">
+        <f t="array" ref="I58">INDEX($B$8:$I$31,INT((ROW(I58)-49)/2)+1,COLUMN(I58)-1)</f>
+        <v>Dmnl</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B59" s="24" t="str" cm="1">
+        <f t="array" ref="B59">IF(MOD(ROW(B58)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B58)-49)/2)+1),"")</f>
+        <v>It is uncertain to what extent bike parking availability will be expanded compared to the current number of bike parking spots per ha of space for cyclists. This uncertainty ranges between zero expansion, and doubling bike parking spots per added space for cyclists.</v>
+      </c>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="24"/>
+      <c r="I59" s="24"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B60" s="1" t="str" cm="1">
+        <f t="array" ref="B60">INDEX($B$8:$I$31,INT((ROW(B60)-49)/2)+1,COLUMN(B60)-1)</f>
         <v>Car adoption</v>
       </c>
-      <c r="C57" s="2" t="str" cm="1">
-        <f t="array" ref="C57">INDEX($B$8:$I$30,INT((ROW(C57)-49)/2)+1,COLUMN(C57)-1)</f>
+      <c r="C60" s="1" t="str" cm="1">
+        <f t="array" ref="C60">INDEX($B$8:$I$31,INT((ROW(C60)-49)/2)+1,COLUMN(C60)-1)</f>
         <v>Vehicle adoption</v>
       </c>
-      <c r="D57" s="2" t="str" cm="1">
-        <f t="array" ref="D57">INDEX($B$8:$I$30,INT((ROW(D57)-49)/2)+1,COLUMN(D57)-1)</f>
+      <c r="D60" s="1" t="str" cm="1">
+        <f t="array" ref="D60">INDEX($B$8:$I$31,INT((ROW(D60)-49)/2)+1,COLUMN(D60)-1)</f>
         <v>constant</v>
       </c>
-      <c r="E57" s="2" t="str" cm="1">
-        <f t="array" ref="E57">INDEX($B$8:$I$30,INT((ROW(E57)-49)/2)+1,COLUMN(E57)-1)</f>
+      <c r="E60" s="1" t="str" cm="1">
+        <f t="array" ref="E60">INDEX($B$8:$I$31,INT((ROW(E60)-49)/2)+1,COLUMN(E60)-1)</f>
         <v>REFERENCE SHIFT IN CAR ADOPTION</v>
       </c>
-      <c r="F57" s="2" cm="1">
-        <f t="array" ref="F57">INDEX($B$8:$I$30,INT((ROW(F57)-49)/2)+1,COLUMN(F57)-1)</f>
+      <c r="F60" s="1" cm="1">
+        <f t="array" ref="F60">INDEX($B$8:$I$31,INT((ROW(F60)-49)/2)+1,COLUMN(F60)-1)</f>
         <v>0.05</v>
       </c>
-      <c r="G57" s="2" cm="1">
-        <f t="array" ref="G57">INDEX($B$8:$I$30,INT((ROW(G57)-49)/2)+1,COLUMN(G57)-1)</f>
+      <c r="G60" s="1" cm="1">
+        <f t="array" ref="G60">INDEX($B$8:$I$31,INT((ROW(G60)-49)/2)+1,COLUMN(G60)-1)</f>
         <v>0.25</v>
       </c>
-      <c r="H57" s="2" cm="1">
-        <f t="array" ref="H57">INDEX($B$8:$I$30,INT((ROW(H57)-49)/2)+1,COLUMN(H57)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I57" s="2" t="str" cm="1">
-        <f t="array" ref="I57">INDEX($B$8:$I$30,INT((ROW(I57)-49)/2)+1,COLUMN(I57)-1)</f>
+      <c r="H60" s="1" cm="1">
+        <f t="array" ref="H60">INDEX($B$8:$I$31,INT((ROW(H60)-49)/2)+1,COLUMN(H60)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I60" s="1" t="str" cm="1">
+        <f t="array" ref="I60">INDEX($B$8:$I$31,INT((ROW(I60)-49)/2)+1,COLUMN(I60)-1)</f>
         <v>Dmnl</v>
       </c>
     </row>
-    <row r="58" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B58" s="3" t="str" cm="1">
-        <f t="array" ref="B58">IF(MOD(ROW(B58)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B58)-49)/2)+1),"")</f>
+    <row r="61" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B61" s="24" t="str" cm="1">
+        <f t="array" ref="B61">IF(MOD(ROW(B60)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B60)-49)/2)+1),"")</f>
         <v>It is uncertain to which extent young adults are currently avoiding car ownership rather than postponing car ownership. A wide range in percentage point shift in car adoption (5 - 25%) is adopted, relative to current adult car adoption</v>
       </c>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
-    </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B59" s="2" t="str" cm="1">
-        <f t="array" ref="B59">INDEX($B$8:$I$30,INT((ROW(B59)-49)/2)+1,COLUMN(B59)-1)</f>
+      <c r="C61" s="24"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="24"/>
+      <c r="H61" s="24"/>
+      <c r="I61" s="24"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B62" s="1" t="str" cm="1">
+        <f t="array" ref="B62">INDEX($B$8:$I$31,INT((ROW(B62)-49)/2)+1,COLUMN(B62)-1)</f>
         <v>Car adoption</v>
       </c>
-      <c r="C59" s="2" t="str" cm="1">
-        <f t="array" ref="C59">INDEX($B$8:$I$30,INT((ROW(C59)-49)/2)+1,COLUMN(C59)-1)</f>
+      <c r="C62" s="1" t="str" cm="1">
+        <f t="array" ref="C62">INDEX($B$8:$I$31,INT((ROW(C62)-49)/2)+1,COLUMN(C62)-1)</f>
         <v>Vehicle adoption</v>
       </c>
-      <c r="D59" s="2" t="str" cm="1">
-        <f t="array" ref="D59">INDEX($B$8:$I$30,INT((ROW(D59)-49)/2)+1,COLUMN(D59)-1)</f>
+      <c r="D62" s="1" t="str" cm="1">
+        <f t="array" ref="D62">INDEX($B$8:$I$31,INT((ROW(D62)-49)/2)+1,COLUMN(D62)-1)</f>
         <v>effect sensitivity</v>
       </c>
-      <c r="E59" s="2" t="str" cm="1">
-        <f t="array" ref="E59">INDEX($B$8:$I$30,INT((ROW(E59)-49)/2)+1,COLUMN(E59)-1)</f>
+      <c r="E62" s="1" t="str" cm="1">
+        <f t="array" ref="E62">INDEX($B$8:$I$31,INT((ROW(E62)-49)/2)+1,COLUMN(E62)-1)</f>
         <v>CAR ADOPTION SENSITIVITY TO USAGE</v>
       </c>
-      <c r="F59" s="2" cm="1">
-        <f t="array" ref="F59">INDEX($B$8:$I$30,INT((ROW(F59)-49)/2)+1,COLUMN(F59)-1)</f>
+      <c r="F62" s="1" cm="1">
+        <f t="array" ref="F62">INDEX($B$8:$I$31,INT((ROW(F62)-49)/2)+1,COLUMN(F62)-1)</f>
         <v>0.5</v>
       </c>
-      <c r="G59" s="2" cm="1">
-        <f t="array" ref="G59">INDEX($B$8:$I$30,INT((ROW(G59)-49)/2)+1,COLUMN(G59)-1)</f>
+      <c r="G62" s="1" cm="1">
+        <f t="array" ref="G62">INDEX($B$8:$I$31,INT((ROW(G62)-49)/2)+1,COLUMN(G62)-1)</f>
         <v>2</v>
       </c>
-      <c r="H59" s="2" cm="1">
-        <f t="array" ref="H59">INDEX($B$8:$I$30,INT((ROW(H59)-49)/2)+1,COLUMN(H59)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I59" s="2" t="str" cm="1">
-        <f t="array" ref="I59">INDEX($B$8:$I$30,INT((ROW(I59)-49)/2)+1,COLUMN(I59)-1)</f>
+      <c r="H62" s="1" cm="1">
+        <f t="array" ref="H62">INDEX($B$8:$I$31,INT((ROW(H62)-49)/2)+1,COLUMN(H62)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I62" s="1" t="str" cm="1">
+        <f t="array" ref="I62">INDEX($B$8:$I$31,INT((ROW(I62)-49)/2)+1,COLUMN(I62)-1)</f>
         <v>Dmnl</v>
       </c>
     </row>
-    <row r="60" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B60" s="3" t="str" cm="1">
-        <f t="array" ref="B60">IF(MOD(ROW(B60)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B60)-49)/2)+1),"")</f>
+    <row r="63" spans="2:9" ht="47.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B63" s="24" t="str" cm="1">
+        <f t="array" ref="B63">IF(MOD(ROW(B62)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B62)-49)/2)+1),"")</f>
         <v>The base assumption is for the current shift in young adult car adoption to vary by 30% if car usage varies by 50% (See Appendix). Since this effect size is uncertain, it is varied by X^y if X is the normalized effect from the base assumption, and y varies between 0.5 and 2.</v>
       </c>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B61" s="2" t="str" cm="1">
-        <f t="array" ref="B61">INDEX($B$8:$I$30,INT((ROW(B61)-49)/2)+1,COLUMN(B61)-1)</f>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="24"/>
+      <c r="H63" s="24"/>
+      <c r="I63" s="24"/>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B64" s="1" t="str" cm="1">
+        <f t="array" ref="B64">INDEX($B$8:$I$31,INT((ROW(B64)-49)/2)+1,COLUMN(B64)-1)</f>
         <v>Bike adoption</v>
       </c>
-      <c r="C61" s="2" t="str" cm="1">
-        <f t="array" ref="C61">INDEX($B$8:$I$30,INT((ROW(C61)-49)/2)+1,COLUMN(C61)-1)</f>
+      <c r="C64" s="1" t="str" cm="1">
+        <f t="array" ref="C64">INDEX($B$8:$I$31,INT((ROW(C64)-49)/2)+1,COLUMN(C64)-1)</f>
         <v>Vehicle adoption</v>
       </c>
-      <c r="D61" s="2" t="str" cm="1">
-        <f t="array" ref="D61">INDEX($B$8:$I$30,INT((ROW(D61)-49)/2)+1,COLUMN(D61)-1)</f>
+      <c r="D64" s="1" t="str" cm="1">
+        <f t="array" ref="D64">INDEX($B$8:$I$31,INT((ROW(D64)-49)/2)+1,COLUMN(D64)-1)</f>
         <v>switch</v>
       </c>
-      <c r="E61" s="2" t="str" cm="1">
-        <f t="array" ref="E61">INDEX($B$8:$I$30,INT((ROW(E61)-49)/2)+1,COLUMN(E61)-1)</f>
+      <c r="E64" s="1" t="str" cm="1">
+        <f t="array" ref="E64">INDEX($B$8:$I$31,INT((ROW(E64)-49)/2)+1,COLUMN(E64)-1)</f>
         <v>TIPPING POINT SWITCH</v>
       </c>
-      <c r="F61" s="2" cm="1">
-        <f t="array" ref="F61">INDEX($B$8:$I$30,INT((ROW(F61)-49)/2)+1,COLUMN(F61)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="G61" s="2" cm="1">
-        <f t="array" ref="G61">INDEX($B$8:$I$30,INT((ROW(G61)-49)/2)+1,COLUMN(G61)-1)</f>
+      <c r="F64" s="1" cm="1">
+        <f t="array" ref="F64">INDEX($B$8:$I$31,INT((ROW(F64)-49)/2)+1,COLUMN(F64)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="G64" s="1" cm="1">
+        <f t="array" ref="G64">INDEX($B$8:$I$31,INT((ROW(G64)-49)/2)+1,COLUMN(G64)-1)</f>
         <v>1</v>
       </c>
-      <c r="H61" s="2" cm="1">
-        <f t="array" ref="H61">INDEX($B$8:$I$30,INT((ROW(H61)-49)/2)+1,COLUMN(H61)-1)</f>
+      <c r="H64" s="1" cm="1">
+        <f t="array" ref="H64">INDEX($B$8:$I$31,INT((ROW(H64)-49)/2)+1,COLUMN(H64)-1)</f>
         <v>1</v>
       </c>
-      <c r="I61" s="2" t="str" cm="1">
-        <f t="array" ref="I61">INDEX($B$8:$I$30,INT((ROW(I61)-49)/2)+1,COLUMN(I61)-1)</f>
+      <c r="I64" s="1" t="str" cm="1">
+        <f t="array" ref="I64">INDEX($B$8:$I$31,INT((ROW(I64)-49)/2)+1,COLUMN(I64)-1)</f>
         <v>Dmnl</v>
       </c>
     </row>
-    <row r="62" spans="2:9" ht="47.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="3" t="str" cm="1">
-        <f t="array" ref="B62">IF(MOD(ROW(B62)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B62)-49)/2)+1),"")</f>
+    <row r="65" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B65" s="24" t="str" cm="1">
+        <f t="array" ref="B65">IF(MOD(ROW(B64)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B64)-49)/2)+1),"")</f>
         <v>Two curves are included in the model that describes how soon the cautious majority becomes receptive to cycling: an early and a late tipping point. The early tipping point assumes the case study is currently at the tipping point, the late tipping point is assumed at an extra 20%-point completion of the cycling network. This assumption is informed by the expert interviews.</v>
       </c>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B63" s="2" t="str" cm="1">
-        <f t="array" ref="B63">INDEX($B$8:$I$30,INT((ROW(B63)-49)/2)+1,COLUMN(B63)-1)</f>
+      <c r="C65" s="24"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="24"/>
+      <c r="G65" s="24"/>
+      <c r="H65" s="24"/>
+      <c r="I65" s="24"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B66" s="1" t="str" cm="1">
+        <f t="array" ref="B66">INDEX($B$8:$I$31,INT((ROW(B66)-49)/2)+1,COLUMN(B66)-1)</f>
         <v>Bike adoption</v>
       </c>
-      <c r="C63" s="2" t="str" cm="1">
-        <f t="array" ref="C63">INDEX($B$8:$I$30,INT((ROW(C63)-49)/2)+1,COLUMN(C63)-1)</f>
+      <c r="C66" s="1" t="str" cm="1">
+        <f t="array" ref="C66">INDEX($B$8:$I$31,INT((ROW(C66)-49)/2)+1,COLUMN(C66)-1)</f>
         <v>Vehicle adoption</v>
       </c>
-      <c r="D63" s="2" t="str" cm="1">
-        <f t="array" ref="D63">INDEX($B$8:$I$30,INT((ROW(D63)-49)/2)+1,COLUMN(D63)-1)</f>
+      <c r="D66" s="1" t="str" cm="1">
+        <f t="array" ref="D66">INDEX($B$8:$I$31,INT((ROW(D66)-49)/2)+1,COLUMN(D66)-1)</f>
         <v>effect sensitivity</v>
       </c>
-      <c r="E63" s="2" t="str" cm="1">
-        <f t="array" ref="E63">INDEX($B$8:$I$30,INT((ROW(E63)-49)/2)+1,COLUMN(E63)-1)</f>
+      <c r="E66" s="1" t="str" cm="1">
+        <f t="array" ref="E66">INDEX($B$8:$I$31,INT((ROW(E66)-49)/2)+1,COLUMN(E66)-1)</f>
         <v>BIKE ADOPTION SENSITIVITY TO PARKING</v>
       </c>
-      <c r="F63" s="2" cm="1">
-        <f t="array" ref="F63">INDEX($B$8:$I$30,INT((ROW(F63)-49)/2)+1,COLUMN(F63)-1)</f>
+      <c r="F66" s="1" cm="1">
+        <f t="array" ref="F66">INDEX($B$8:$I$31,INT((ROW(F66)-49)/2)+1,COLUMN(F66)-1)</f>
         <v>0.5</v>
       </c>
-      <c r="G63" s="2" cm="1">
-        <f t="array" ref="G63">INDEX($B$8:$I$30,INT((ROW(G63)-49)/2)+1,COLUMN(G63)-1)</f>
+      <c r="G66" s="1" cm="1">
+        <f t="array" ref="G66">INDEX($B$8:$I$31,INT((ROW(G66)-49)/2)+1,COLUMN(G66)-1)</f>
         <v>2</v>
       </c>
-      <c r="H63" s="2" cm="1">
-        <f t="array" ref="H63">INDEX($B$8:$I$30,INT((ROW(H63)-49)/2)+1,COLUMN(H63)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I63" s="2" t="str" cm="1">
-        <f t="array" ref="I63">INDEX($B$8:$I$30,INT((ROW(I63)-49)/2)+1,COLUMN(I63)-1)</f>
+      <c r="H66" s="1" cm="1">
+        <f t="array" ref="H66">INDEX($B$8:$I$31,INT((ROW(H66)-49)/2)+1,COLUMN(H66)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I66" s="1" t="str" cm="1">
+        <f t="array" ref="I66">INDEX($B$8:$I$31,INT((ROW(I66)-49)/2)+1,COLUMN(I66)-1)</f>
         <v>Dmnl</v>
       </c>
     </row>
-    <row r="64" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B64" s="3" t="str" cm="1">
-        <f t="array" ref="B64">IF(MOD(ROW(B64)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B64)-49)/2)+1),"")</f>
+    <row r="67" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B67" s="24" t="str" cm="1">
+        <f t="array" ref="B67">IF(MOD(ROW(B66)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B66)-49)/2)+1),"")</f>
         <v>The base assumption is for bike usage and bike parking availability together to multiply the reference contact fruitfulness (0.02) by up to 4 times (see Appendix ). Since this effect size is uncertain, it is varied by X^y if X is the normalized effect from the base assumption, and y varies between 0.5 and 2.</v>
       </c>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
-    </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B65" s="2" t="str" cm="1">
-        <f t="array" ref="B65">INDEX($B$8:$I$30,INT((ROW(B65)-49)/2)+1,COLUMN(B65)-1)</f>
+      <c r="C67" s="24"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="24"/>
+      <c r="H67" s="24"/>
+      <c r="I67" s="24"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B68" s="1" t="str" cm="1">
+        <f t="array" ref="B68">INDEX($B$8:$I$31,INT((ROW(B68)-49)/2)+1,COLUMN(B68)-1)</f>
         <v>Bike adoption</v>
       </c>
-      <c r="C65" s="2" t="str" cm="1">
-        <f t="array" ref="C65">INDEX($B$8:$I$30,INT((ROW(C65)-49)/2)+1,COLUMN(C65)-1)</f>
+      <c r="C68" s="1" t="str" cm="1">
+        <f t="array" ref="C68">INDEX($B$8:$I$31,INT((ROW(C68)-49)/2)+1,COLUMN(C68)-1)</f>
         <v>Vehicle adoption</v>
       </c>
-      <c r="D65" s="2" t="str" cm="1">
-        <f t="array" ref="D65">INDEX($B$8:$I$30,INT((ROW(D65)-49)/2)+1,COLUMN(D65)-1)</f>
+      <c r="D68" s="1" t="str" cm="1">
+        <f t="array" ref="D68">INDEX($B$8:$I$31,INT((ROW(D68)-49)/2)+1,COLUMN(D68)-1)</f>
         <v>effect sensitivity</v>
       </c>
-      <c r="E65" s="2" t="str" cm="1">
-        <f t="array" ref="E65">INDEX($B$8:$I$30,INT((ROW(E65)-49)/2)+1,COLUMN(E65)-1)</f>
+      <c r="E68" s="1" t="str" cm="1">
+        <f t="array" ref="E68">INDEX($B$8:$I$31,INT((ROW(E68)-49)/2)+1,COLUMN(E68)-1)</f>
         <v>BIKE ADOPTION SENSITIVITY TO USAGE</v>
       </c>
-      <c r="F65" s="2" cm="1">
-        <f t="array" ref="F65">INDEX($B$8:$I$30,INT((ROW(F65)-49)/2)+1,COLUMN(F65)-1)</f>
+      <c r="F68" s="1" cm="1">
+        <f t="array" ref="F68">INDEX($B$8:$I$31,INT((ROW(F68)-49)/2)+1,COLUMN(F68)-1)</f>
         <v>0.5</v>
       </c>
-      <c r="G65" s="2" cm="1">
-        <f t="array" ref="G65">INDEX($B$8:$I$30,INT((ROW(G65)-49)/2)+1,COLUMN(G65)-1)</f>
+      <c r="G68" s="1" cm="1">
+        <f t="array" ref="G68">INDEX($B$8:$I$31,INT((ROW(G68)-49)/2)+1,COLUMN(G68)-1)</f>
         <v>2</v>
       </c>
-      <c r="H65" s="2" cm="1">
-        <f t="array" ref="H65">INDEX($B$8:$I$30,INT((ROW(H65)-49)/2)+1,COLUMN(H65)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I65" s="2" t="str" cm="1">
-        <f t="array" ref="I65">INDEX($B$8:$I$30,INT((ROW(I65)-49)/2)+1,COLUMN(I65)-1)</f>
+      <c r="H68" s="1" cm="1">
+        <f t="array" ref="H68">INDEX($B$8:$I$31,INT((ROW(H68)-49)/2)+1,COLUMN(H68)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I68" s="1" t="str" cm="1">
+        <f t="array" ref="I68">INDEX($B$8:$I$31,INT((ROW(I68)-49)/2)+1,COLUMN(I68)-1)</f>
         <v>Dmnl</v>
       </c>
     </row>
-    <row r="66" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B66" s="3" t="str" cm="1">
-        <f t="array" ref="B66">IF(MOD(ROW(B66)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B66)-49)/2)+1),"")</f>
+    <row r="69" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B69" s="24" t="str" cm="1">
+        <f t="array" ref="B69">IF(MOD(ROW(B68)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B68)-49)/2)+1),"")</f>
         <v>The base assumption is for bike usage and bike parking availability together to multiply the reference contact fruitfulness (0.02) by up to 4 times (see Appendix ). Since this effect size is uncertain, it is varied by X^y if X is the normalized effect from the base assumption, and y varies between 0.5 and 2.</v>
       </c>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
-    </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B67" s="2" t="str" cm="1">
-        <f t="array" ref="B67">INDEX($B$8:$I$30,INT((ROW(B67)-49)/2)+1,COLUMN(B67)-1)</f>
+      <c r="C69" s="24"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="24"/>
+      <c r="H69" s="24"/>
+      <c r="I69" s="24"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B70" s="1" t="str" cm="1">
+        <f t="array" ref="B70">INDEX($B$8:$I$31,INT((ROW(B70)-49)/2)+1,COLUMN(B70)-1)</f>
         <v>Bike adoption</v>
       </c>
-      <c r="C67" s="2" t="str" cm="1">
-        <f t="array" ref="C67">INDEX($B$8:$I$30,INT((ROW(C67)-49)/2)+1,COLUMN(C67)-1)</f>
+      <c r="C70" s="1" t="str" cm="1">
+        <f t="array" ref="C70">INDEX($B$8:$I$31,INT((ROW(C70)-49)/2)+1,COLUMN(C70)-1)</f>
         <v>Vehicle adoption</v>
       </c>
-      <c r="D67" s="2" t="str" cm="1">
-        <f t="array" ref="D67">INDEX($B$8:$I$30,INT((ROW(D67)-49)/2)+1,COLUMN(D67)-1)</f>
+      <c r="D70" s="1" t="str" cm="1">
+        <f t="array" ref="D70">INDEX($B$8:$I$31,INT((ROW(D70)-49)/2)+1,COLUMN(D70)-1)</f>
         <v>constant</v>
       </c>
-      <c r="E67" s="2" t="str" cm="1">
-        <f t="array" ref="E67">INDEX($B$8:$I$30,INT((ROW(E67)-49)/2)+1,COLUMN(E67)-1)</f>
+      <c r="E70" s="1" t="str" cm="1">
+        <f t="array" ref="E70">INDEX($B$8:$I$31,INT((ROW(E70)-49)/2)+1,COLUMN(E70)-1)</f>
         <v>CONTACT RATE</v>
       </c>
-      <c r="F67" s="2" cm="1">
-        <f t="array" ref="F67">INDEX($B$8:$I$30,INT((ROW(F67)-49)/2)+1,COLUMN(F67)-1)</f>
+      <c r="F70" s="1" cm="1">
+        <f t="array" ref="F70">INDEX($B$8:$I$31,INT((ROW(F70)-49)/2)+1,COLUMN(F70)-1)</f>
         <v>1</v>
       </c>
-      <c r="G67" s="2" cm="1">
-        <f t="array" ref="G67">INDEX($B$8:$I$30,INT((ROW(G67)-49)/2)+1,COLUMN(G67)-1)</f>
+      <c r="G70" s="1" cm="1">
+        <f t="array" ref="G70">INDEX($B$8:$I$31,INT((ROW(G70)-49)/2)+1,COLUMN(G70)-1)</f>
         <v>3</v>
       </c>
-      <c r="H67" s="2" cm="1">
-        <f t="array" ref="H67">INDEX($B$8:$I$30,INT((ROW(H67)-49)/2)+1,COLUMN(H67)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I67" s="2" t="str" cm="1">
-        <f t="array" ref="I67">INDEX($B$8:$I$30,INT((ROW(I67)-49)/2)+1,COLUMN(I67)-1)</f>
+      <c r="H70" s="1" cm="1">
+        <f t="array" ref="H70">INDEX($B$8:$I$31,INT((ROW(H70)-49)/2)+1,COLUMN(H70)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I70" s="1" t="str" cm="1">
+        <f t="array" ref="I70">INDEX($B$8:$I$31,INT((ROW(I70)-49)/2)+1,COLUMN(I70)-1)</f>
         <v>Dmnl</v>
       </c>
     </row>
-    <row r="68" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B68" s="3" t="str" cm="1">
-        <f t="array" ref="B68">IF(MOD(ROW(B68)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B68)-49)/2)+1),"")</f>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B71" s="24" t="str" cm="1">
+        <f t="array" ref="B71">IF(MOD(ROW(B70)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B70)-49)/2)+1),"")</f>
         <v>The contact rate (number of unique, high-quality social contacts per person per year) is uncertain, although in urban areas it tends to be high (\citep{}). A wide range is chosen of 3 - 7.</v>
       </c>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
-    </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B69" s="2" t="str" cm="1">
-        <f t="array" ref="B69">INDEX($B$8:$I$30,INT((ROW(B69)-49)/2)+1,COLUMN(B69)-1)</f>
+      <c r="C71" s="24"/>
+      <c r="D71" s="24"/>
+      <c r="E71" s="24"/>
+      <c r="F71" s="24"/>
+      <c r="G71" s="24"/>
+      <c r="H71" s="24"/>
+      <c r="I71" s="24"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B72" s="1" t="str" cm="1">
+        <f t="array" ref="B72">INDEX($B$8:$I$31,INT((ROW(B72)-49)/2)+1,COLUMN(B72)-1)</f>
         <v>Bike adoption</v>
       </c>
-      <c r="C69" s="2" t="str" cm="1">
-        <f t="array" ref="C69">INDEX($B$8:$I$30,INT((ROW(C69)-49)/2)+1,COLUMN(C69)-1)</f>
+      <c r="C72" s="1" t="str" cm="1">
+        <f t="array" ref="C72">INDEX($B$8:$I$31,INT((ROW(C72)-49)/2)+1,COLUMN(C72)-1)</f>
         <v>Vehicle adoption</v>
       </c>
-      <c r="D69" s="2" t="str" cm="1">
-        <f t="array" ref="D69">INDEX($B$8:$I$30,INT((ROW(D69)-49)/2)+1,COLUMN(D69)-1)</f>
+      <c r="D72" s="1" t="str" cm="1">
+        <f t="array" ref="D72">INDEX($B$8:$I$31,INT((ROW(D72)-49)/2)+1,COLUMN(D72)-1)</f>
         <v>constant</v>
       </c>
-      <c r="E69" s="2" t="str" cm="1">
-        <f t="array" ref="E69">INDEX($B$8:$I$30,INT((ROW(E69)-49)/2)+1,COLUMN(E69)-1)</f>
+      <c r="E72" s="1" t="str" cm="1">
+        <f t="array" ref="E72">INDEX($B$8:$I$31,INT((ROW(E72)-49)/2)+1,COLUMN(E72)-1)</f>
         <v>BIKESHARING TO PRIVATE BIKE UPGRADE FRACTION</v>
       </c>
-      <c r="F69" s="2" cm="1">
-        <f t="array" ref="F69">INDEX($B$8:$I$30,INT((ROW(F69)-49)/2)+1,COLUMN(F69)-1)</f>
+      <c r="F72" s="1" cm="1">
+        <f t="array" ref="F72">INDEX($B$8:$I$31,INT((ROW(F72)-49)/2)+1,COLUMN(F72)-1)</f>
         <v>0.05</v>
       </c>
-      <c r="G69" s="2" cm="1">
-        <f t="array" ref="G69">INDEX($B$8:$I$30,INT((ROW(G69)-49)/2)+1,COLUMN(G69)-1)</f>
+      <c r="G72" s="1" cm="1">
+        <f t="array" ref="G72">INDEX($B$8:$I$31,INT((ROW(G72)-49)/2)+1,COLUMN(G72)-1)</f>
         <v>0.25</v>
       </c>
-      <c r="H69" s="2" cm="1">
-        <f t="array" ref="H69">INDEX($B$8:$I$30,INT((ROW(H69)-49)/2)+1,COLUMN(H69)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I69" s="2" t="str" cm="1">
-        <f t="array" ref="I69">INDEX($B$8:$I$30,INT((ROW(I69)-49)/2)+1,COLUMN(I69)-1)</f>
+      <c r="H72" s="1" cm="1">
+        <f t="array" ref="H72">INDEX($B$8:$I$31,INT((ROW(H72)-49)/2)+1,COLUMN(H72)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I72" s="1" t="str" cm="1">
+        <f t="array" ref="I72">INDEX($B$8:$I$31,INT((ROW(I72)-49)/2)+1,COLUMN(I72)-1)</f>
         <v>Dmnl</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B70" s="3" t="str" cm="1">
-        <f t="array" ref="B70">IF(MOD(ROW(B70)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B70)-49)/2)+1),"")</f>
+    <row r="73" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B73" s="24" t="str" cm="1">
+        <f t="array" ref="B73">IF(MOD(ROW(B72)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B72)-49)/2)+1),"")</f>
         <v>The share of bikesharing users upgrading to private bike use after two years is uncertain. A wide range is assumed of 5 - 25%.</v>
       </c>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-      <c r="I70" s="3"/>
-    </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B71" s="2" t="str" cm="1">
-        <f t="array" ref="B71">INDEX($B$8:$I$30,INT((ROW(B71)-49)/2)+1,COLUMN(B71)-1)</f>
+      <c r="C73" s="24"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="24"/>
+      <c r="H73" s="24"/>
+      <c r="I73" s="24"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B74" s="1" t="str" cm="1">
+        <f t="array" ref="B74">INDEX($B$8:$I$31,INT((ROW(B74)-49)/2)+1,COLUMN(B74)-1)</f>
         <v>Bike adoption</v>
       </c>
-      <c r="C71" s="2" t="str" cm="1">
-        <f t="array" ref="C71">INDEX($B$8:$I$30,INT((ROW(C71)-49)/2)+1,COLUMN(C71)-1)</f>
+      <c r="C74" s="1" t="str" cm="1">
+        <f t="array" ref="C74">INDEX($B$8:$I$31,INT((ROW(C74)-49)/2)+1,COLUMN(C74)-1)</f>
         <v>Vehicle adoption</v>
       </c>
-      <c r="D71" s="2" t="str" cm="1">
-        <f t="array" ref="D71">INDEX($B$8:$I$30,INT((ROW(D71)-49)/2)+1,COLUMN(D71)-1)</f>
+      <c r="D74" s="1" t="str" cm="1">
+        <f t="array" ref="D74">INDEX($B$8:$I$31,INT((ROW(D74)-49)/2)+1,COLUMN(D74)-1)</f>
         <v>switch</v>
       </c>
-      <c r="E71" s="2" t="str" cm="1">
-        <f t="array" ref="E71">INDEX($B$8:$I$30,INT((ROW(E71)-49)/2)+1,COLUMN(E71)-1)</f>
+      <c r="E74" s="1" t="str" cm="1">
+        <f t="array" ref="E74">INDEX($B$8:$I$31,INT((ROW(E74)-49)/2)+1,COLUMN(E74)-1)</f>
         <v>EBIKE UPTAKE SWITCH</v>
       </c>
-      <c r="F71" s="2" cm="1">
-        <f t="array" ref="F71">INDEX($B$8:$I$30,INT((ROW(F71)-49)/2)+1,COLUMN(F71)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="G71" s="2" cm="1">
-        <f t="array" ref="G71">INDEX($B$8:$I$30,INT((ROW(G71)-49)/2)+1,COLUMN(G71)-1)</f>
+      <c r="F74" s="1" cm="1">
+        <f t="array" ref="F74">INDEX($B$8:$I$31,INT((ROW(F74)-49)/2)+1,COLUMN(F74)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="G74" s="1" cm="1">
+        <f t="array" ref="G74">INDEX($B$8:$I$31,INT((ROW(G74)-49)/2)+1,COLUMN(G74)-1)</f>
         <v>1</v>
       </c>
-      <c r="H71" s="2" cm="1">
-        <f t="array" ref="H71">INDEX($B$8:$I$30,INT((ROW(H71)-49)/2)+1,COLUMN(H71)-1)</f>
+      <c r="H74" s="1" cm="1">
+        <f t="array" ref="H74">INDEX($B$8:$I$31,INT((ROW(H74)-49)/2)+1,COLUMN(H74)-1)</f>
         <v>1</v>
       </c>
-      <c r="I71" s="2" t="str" cm="1">
-        <f t="array" ref="I71">INDEX($B$8:$I$30,INT((ROW(I71)-49)/2)+1,COLUMN(I71)-1)</f>
+      <c r="I74" s="1" t="str" cm="1">
+        <f t="array" ref="I74">INDEX($B$8:$I$31,INT((ROW(I74)-49)/2)+1,COLUMN(I74)-1)</f>
         <v>Dmnl</v>
       </c>
     </row>
-    <row r="72" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B72" s="3" t="str" cm="1">
-        <f t="array" ref="B72">IF(MOD(ROW(B72)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B72)-49)/2)+1),"")</f>
+    <row r="75" spans="2:9" ht="43.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B75" s="24" t="str" cm="1">
+        <f t="array" ref="B75">IF(MOD(ROW(B74)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B74)-49)/2)+1),"")</f>
         <v>The pace and final state of e-bike uptake is uncertain. The model varies between two discrete scenarios, both starting from the current level of adoption, but continuing at different speeds and until different final states (see Appendix )</v>
       </c>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
-    </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B73" s="2" t="str" cm="1">
-        <f t="array" ref="B73">INDEX($B$8:$I$30,INT((ROW(B73)-49)/2)+1,COLUMN(B73)-1)</f>
+      <c r="C75" s="24"/>
+      <c r="D75" s="24"/>
+      <c r="E75" s="24"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="24"/>
+      <c r="H75" s="24"/>
+      <c r="I75" s="24"/>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B76" s="1" t="str" cm="1">
+        <f t="array" ref="B76">INDEX($B$8:$I$31,INT((ROW(B76)-49)/2)+1,COLUMN(B76)-1)</f>
         <v>Mode choice</v>
       </c>
-      <c r="C73" s="2" t="str" cm="1">
-        <f t="array" ref="C73">INDEX($B$8:$I$30,INT((ROW(C73)-49)/2)+1,COLUMN(C73)-1)</f>
+      <c r="C76" s="1" t="str" cm="1">
+        <f t="array" ref="C76">INDEX($B$8:$I$31,INT((ROW(C76)-49)/2)+1,COLUMN(C76)-1)</f>
         <v>Mode choice</v>
       </c>
-      <c r="D73" s="2" t="str" cm="1">
-        <f t="array" ref="D73">INDEX($B$8:$I$30,INT((ROW(D73)-49)/2)+1,COLUMN(D73)-1)</f>
+      <c r="D76" s="1" t="str" cm="1">
+        <f t="array" ref="D76">INDEX($B$8:$I$31,INT((ROW(D76)-49)/2)+1,COLUMN(D76)-1)</f>
         <v>effect sensitivity</v>
       </c>
-      <c r="E73" s="2" t="str" cm="1">
-        <f t="array" ref="E73">INDEX($B$8:$I$30,INT((ROW(E73)-49)/2)+1,COLUMN(E73)-1)</f>
+      <c r="E76" s="1" t="str" cm="1">
+        <f t="array" ref="E76">INDEX($B$8:$I$31,INT((ROW(E76)-49)/2)+1,COLUMN(E76)-1)</f>
         <v>CAR NETWORK DISTANCE SENSITIVITY</v>
       </c>
-      <c r="F73" s="2" cm="1">
-        <f t="array" ref="F73">INDEX($B$8:$I$30,INT((ROW(F73)-49)/2)+1,COLUMN(F73)-1)</f>
+      <c r="F76" s="1" cm="1">
+        <f t="array" ref="F76">INDEX($B$8:$I$31,INT((ROW(F76)-49)/2)+1,COLUMN(F76)-1)</f>
         <v>0.5</v>
       </c>
-      <c r="G73" s="2" cm="1">
-        <f t="array" ref="G73">INDEX($B$8:$I$30,INT((ROW(G73)-49)/2)+1,COLUMN(G73)-1)</f>
+      <c r="G76" s="1" cm="1">
+        <f t="array" ref="G76">INDEX($B$8:$I$31,INT((ROW(G76)-49)/2)+1,COLUMN(G76)-1)</f>
         <v>2</v>
       </c>
-      <c r="H73" s="2" cm="1">
-        <f t="array" ref="H73">INDEX($B$8:$I$30,INT((ROW(H73)-49)/2)+1,COLUMN(H73)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I73" s="2" t="str" cm="1">
-        <f t="array" ref="I73">INDEX($B$8:$I$30,INT((ROW(I73)-49)/2)+1,COLUMN(I73)-1)</f>
+      <c r="H76" s="1" cm="1">
+        <f t="array" ref="H76">INDEX($B$8:$I$31,INT((ROW(H76)-49)/2)+1,COLUMN(H76)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I76" s="1" t="str" cm="1">
+        <f t="array" ref="I76">INDEX($B$8:$I$31,INT((ROW(I76)-49)/2)+1,COLUMN(I76)-1)</f>
         <v>Dmnl</v>
       </c>
     </row>
-    <row r="74" spans="2:9" ht="43.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B74" s="3" t="str" cm="1">
-        <f t="array" ref="B74">IF(MOD(ROW(B74)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B74)-49)/2)+1),"")</f>
+    <row r="77" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B77" s="24" t="str" cm="1">
+        <f t="array" ref="B77">IF(MOD(ROW(B76)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B76)-49)/2)+1),"")</f>
         <v>The base assumption is for the car network distance to euclidian distance ratio to increase to 1.8 when only half of the network is car-accessible, and decrease to 1.1 if average car lanes per road becomes 4 (see Appendix ). Since this effect size is uncertain, it is varied by X^y if X is the normalized effect from the base assumption, and y varies between 0.5 and 2.</v>
       </c>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-    </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B75" s="2" t="str" cm="1">
-        <f t="array" ref="B75">INDEX($B$8:$I$30,INT((ROW(B75)-49)/2)+1,COLUMN(B75)-1)</f>
+      <c r="C77" s="24"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="24"/>
+      <c r="G77" s="24"/>
+      <c r="H77" s="24"/>
+      <c r="I77" s="24"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B78" s="1" t="str" cm="1">
+        <f t="array" ref="B78">INDEX($B$8:$I$31,INT((ROW(B78)-49)/2)+1,COLUMN(B78)-1)</f>
         <v>Mode choice</v>
       </c>
-      <c r="C75" s="2" t="str" cm="1">
-        <f t="array" ref="C75">INDEX($B$8:$I$30,INT((ROW(C75)-49)/2)+1,COLUMN(C75)-1)</f>
+      <c r="C78" s="1" t="str" cm="1">
+        <f t="array" ref="C78">INDEX($B$8:$I$31,INT((ROW(C78)-49)/2)+1,COLUMN(C78)-1)</f>
         <v>Mode choice</v>
       </c>
-      <c r="D75" s="2" t="str" cm="1">
-        <f t="array" ref="D75">INDEX($B$8:$I$30,INT((ROW(D75)-49)/2)+1,COLUMN(D75)-1)</f>
+      <c r="D78" s="1" t="str" cm="1">
+        <f t="array" ref="D78">INDEX($B$8:$I$31,INT((ROW(D78)-49)/2)+1,COLUMN(D78)-1)</f>
         <v>effect sensitivity</v>
       </c>
-      <c r="E75" s="2" t="str" cm="1">
-        <f t="array" ref="E75">INDEX($B$8:$I$30,INT((ROW(E75)-49)/2)+1,COLUMN(E75)-1)</f>
+      <c r="E78" s="1" t="str" cm="1">
+        <f t="array" ref="E78">INDEX($B$8:$I$31,INT((ROW(E78)-49)/2)+1,COLUMN(E78)-1)</f>
         <v>CYCLING NETWORK DISTANCE SENSITIVITY</v>
       </c>
-      <c r="F75" s="2" cm="1">
-        <f t="array" ref="F75">INDEX($B$8:$I$30,INT((ROW(F75)-49)/2)+1,COLUMN(F75)-1)</f>
+      <c r="F78" s="1" cm="1">
+        <f t="array" ref="F78">INDEX($B$8:$I$31,INT((ROW(F78)-49)/2)+1,COLUMN(F78)-1)</f>
         <v>0.5</v>
       </c>
-      <c r="G75" s="2" cm="1">
-        <f t="array" ref="G75">INDEX($B$8:$I$30,INT((ROW(G75)-49)/2)+1,COLUMN(G75)-1)</f>
+      <c r="G78" s="1" cm="1">
+        <f t="array" ref="G78">INDEX($B$8:$I$31,INT((ROW(G78)-49)/2)+1,COLUMN(G78)-1)</f>
         <v>2</v>
       </c>
-      <c r="H75" s="2" cm="1">
-        <f t="array" ref="H75">INDEX($B$8:$I$30,INT((ROW(H75)-49)/2)+1,COLUMN(H75)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I75" s="2" t="str" cm="1">
-        <f t="array" ref="I75">INDEX($B$8:$I$30,INT((ROW(I75)-49)/2)+1,COLUMN(I75)-1)</f>
+      <c r="H78" s="1" cm="1">
+        <f t="array" ref="H78">INDEX($B$8:$I$31,INT((ROW(H78)-49)/2)+1,COLUMN(H78)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I78" s="1" t="str" cm="1">
+        <f t="array" ref="I78">INDEX($B$8:$I$31,INT((ROW(I78)-49)/2)+1,COLUMN(I78)-1)</f>
         <v>Dmnl</v>
       </c>
     </row>
-    <row r="76" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B76" s="3" t="str" cm="1">
-        <f t="array" ref="B76">IF(MOD(ROW(B76)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B76)-49)/2)+1),"")</f>
+    <row r="79" spans="2:9" ht="44.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B79" s="24" t="str" cm="1">
+        <f t="array" ref="B79">IF(MOD(ROW(B78)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B78)-49)/2)+1),"")</f>
         <v xml:space="preserve">The base assumption is for distance to euclidian distance ratio to double when zero roads have bike lanes, and to fall to 1.1 when all roads have bike lanes (see Appendix ). Since this effect size is uncertain, it is varied by X^y if X is the normalized effect from the base assumption, and y varies between 0.5 and 2. </v>
       </c>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
-      <c r="H76" s="3"/>
-      <c r="I76" s="3"/>
-    </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B77" s="2" t="str" cm="1">
-        <f t="array" ref="B77">INDEX($B$8:$I$30,INT((ROW(B77)-49)/2)+1,COLUMN(B77)-1)</f>
+      <c r="C79" s="24"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="24"/>
+      <c r="H79" s="24"/>
+      <c r="I79" s="24"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B80" s="1" t="str" cm="1">
+        <f t="array" ref="B80">INDEX($B$8:$I$31,INT((ROW(B80)-49)/2)+1,COLUMN(B80)-1)</f>
         <v>Mode choice</v>
       </c>
-      <c r="C77" s="2" t="str" cm="1">
-        <f t="array" ref="C77">INDEX($B$8:$I$30,INT((ROW(C77)-49)/2)+1,COLUMN(C77)-1)</f>
+      <c r="C80" s="1" t="str" cm="1">
+        <f t="array" ref="C80">INDEX($B$8:$I$31,INT((ROW(C80)-49)/2)+1,COLUMN(C80)-1)</f>
         <v>Mode choice</v>
       </c>
-      <c r="D77" s="2" t="str" cm="1">
-        <f t="array" ref="D77">INDEX($B$8:$I$30,INT((ROW(D77)-49)/2)+1,COLUMN(D77)-1)</f>
+      <c r="D80" s="1" t="str" cm="1">
+        <f t="array" ref="D80">INDEX($B$8:$I$31,INT((ROW(D80)-49)/2)+1,COLUMN(D80)-1)</f>
         <v>effect sensitivity</v>
       </c>
-      <c r="E77" s="2" t="str" cm="1">
-        <f t="array" ref="E77">INDEX($B$8:$I$30,INT((ROW(E77)-49)/2)+1,COLUMN(E77)-1)</f>
+      <c r="E80" s="1" t="str" cm="1">
+        <f t="array" ref="E80">INDEX($B$8:$I$31,INT((ROW(E80)-49)/2)+1,COLUMN(E80)-1)</f>
         <v>SUBJECTIVE CYCLING TIME SENSITIVITY</v>
       </c>
-      <c r="F77" s="2" cm="1">
-        <f t="array" ref="F77">INDEX($B$8:$I$30,INT((ROW(F77)-49)/2)+1,COLUMN(F77)-1)</f>
+      <c r="F80" s="1" cm="1">
+        <f t="array" ref="F80">INDEX($B$8:$I$31,INT((ROW(F80)-49)/2)+1,COLUMN(F80)-1)</f>
         <v>0.5</v>
       </c>
-      <c r="G77" s="2" cm="1">
-        <f t="array" ref="G77">INDEX($B$8:$I$30,INT((ROW(G77)-49)/2)+1,COLUMN(G77)-1)</f>
+      <c r="G80" s="1" cm="1">
+        <f t="array" ref="G80">INDEX($B$8:$I$31,INT((ROW(G80)-49)/2)+1,COLUMN(G80)-1)</f>
         <v>2</v>
       </c>
-      <c r="H77" s="2" cm="1">
-        <f t="array" ref="H77">INDEX($B$8:$I$30,INT((ROW(H77)-49)/2)+1,COLUMN(H77)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I77" s="2" t="str" cm="1">
-        <f t="array" ref="I77">INDEX($B$8:$I$30,INT((ROW(I77)-49)/2)+1,COLUMN(I77)-1)</f>
+      <c r="H80" s="1" cm="1">
+        <f t="array" ref="H80">INDEX($B$8:$I$31,INT((ROW(H80)-49)/2)+1,COLUMN(H80)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I80" s="1" t="str" cm="1">
+        <f t="array" ref="I80">INDEX($B$8:$I$31,INT((ROW(I80)-49)/2)+1,COLUMN(I80)-1)</f>
         <v>Dmnl</v>
       </c>
     </row>
-    <row r="78" spans="2:9" ht="44.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B78" s="3" t="str" cm="1">
-        <f t="array" ref="B78">IF(MOD(ROW(B78)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B78)-49)/2)+1),"")</f>
+    <row r="81" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B81" s="24" t="str" cm="1">
+        <f t="array" ref="B81">IF(MOD(ROW(B80)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B80)-49)/2)+1),"")</f>
         <v>The base assumption is for subjective cost of cycling to vary by a maximum of 0.8 Minutes per Minute (In the most extreme scenario, where three additive effects stack up. This is not plausible and does not occur in any of the experiments.) (see Appendix ). Since this effect size is uncertain, it is varied by X*y if X is the subjective value factor, and y varies between 0.5 and 1.5.</v>
       </c>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-      <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
-    </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B79" s="2" t="str" cm="1">
-        <f t="array" ref="B79">INDEX($B$8:$I$30,INT((ROW(B79)-49)/2)+1,COLUMN(B79)-1)</f>
+      <c r="C81" s="24"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="24"/>
+      <c r="H81" s="24"/>
+      <c r="I81" s="24"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B82" s="1" t="str" cm="1">
+        <f t="array" ref="B82">INDEX($B$8:$I$31,INT((ROW(B82)-49)/2)+1,COLUMN(B82)-1)</f>
         <v>Mode choice</v>
       </c>
-      <c r="C79" s="2" t="str" cm="1">
-        <f t="array" ref="C79">INDEX($B$8:$I$30,INT((ROW(C79)-49)/2)+1,COLUMN(C79)-1)</f>
+      <c r="C82" s="1" t="str" cm="1">
+        <f t="array" ref="C82">INDEX($B$8:$I$31,INT((ROW(C82)-49)/2)+1,COLUMN(C82)-1)</f>
         <v>Mode choice</v>
       </c>
-      <c r="D79" s="2" t="str" cm="1">
-        <f t="array" ref="D79">INDEX($B$8:$I$30,INT((ROW(D79)-49)/2)+1,COLUMN(D79)-1)</f>
+      <c r="D82" s="1" t="str" cm="1">
+        <f t="array" ref="D82">INDEX($B$8:$I$31,INT((ROW(D82)-49)/2)+1,COLUMN(D82)-1)</f>
         <v>effect sensitivity</v>
       </c>
-      <c r="E79" s="2" t="str" cm="1">
-        <f t="array" ref="E79">INDEX($B$8:$I$30,INT((ROW(E79)-49)/2)+1,COLUMN(E79)-1)</f>
+      <c r="E82" s="1" t="str" cm="1">
+        <f t="array" ref="E82">INDEX($B$8:$I$31,INT((ROW(E82)-49)/2)+1,COLUMN(E82)-1)</f>
         <v>PARKING SEARCH AND EGRESS SENSITIVITY</v>
       </c>
-      <c r="F79" s="2" cm="1">
-        <f t="array" ref="F79">INDEX($B$8:$I$30,INT((ROW(F79)-49)/2)+1,COLUMN(F79)-1)</f>
+      <c r="F82" s="1" cm="1">
+        <f t="array" ref="F82">INDEX($B$8:$I$31,INT((ROW(F82)-49)/2)+1,COLUMN(F82)-1)</f>
         <v>0.5</v>
       </c>
-      <c r="G79" s="2" cm="1">
-        <f t="array" ref="G79">INDEX($B$8:$I$30,INT((ROW(G79)-49)/2)+1,COLUMN(G79)-1)</f>
+      <c r="G82" s="1" cm="1">
+        <f t="array" ref="G82">INDEX($B$8:$I$31,INT((ROW(G82)-49)/2)+1,COLUMN(G82)-1)</f>
         <v>2</v>
       </c>
-      <c r="H79" s="2" cm="1">
-        <f t="array" ref="H79">INDEX($B$8:$I$30,INT((ROW(H79)-49)/2)+1,COLUMN(H79)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I79" s="2" t="str" cm="1">
-        <f t="array" ref="I79">INDEX($B$8:$I$30,INT((ROW(I79)-49)/2)+1,COLUMN(I79)-1)</f>
+      <c r="H82" s="1" cm="1">
+        <f t="array" ref="H82">INDEX($B$8:$I$31,INT((ROW(H82)-49)/2)+1,COLUMN(H82)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I82" s="1" t="str" cm="1">
+        <f t="array" ref="I82">INDEX($B$8:$I$31,INT((ROW(I82)-49)/2)+1,COLUMN(I82)-1)</f>
         <v>Dmnl</v>
       </c>
     </row>
-    <row r="80" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B80" s="3" t="str" cm="1">
-        <f t="array" ref="B80">IF(MOD(ROW(B80)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B80)-49)/2)+1),"")</f>
+    <row r="83" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B83" s="24" t="str" cm="1">
+        <f t="array" ref="B83">IF(MOD(ROW(B82)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B82)-49)/2)+1),"")</f>
         <v>The base assumption is for parking search and egress time to vary between  5 and 14 minutes depending on city parking per city car (see Appendix ). Since this effect size is uncertain, it is varied by X^y if X is the normalized effect from the base assumption, and y varies between 0.5 and 2.</v>
       </c>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
-      <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-    </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B81" s="2" t="str" cm="1">
-        <f t="array" ref="B81">INDEX($B$8:$I$30,INT((ROW(B81)-49)/2)+1,COLUMN(B81)-1)</f>
+      <c r="C83" s="24"/>
+      <c r="D83" s="24"/>
+      <c r="E83" s="24"/>
+      <c r="F83" s="24"/>
+      <c r="G83" s="24"/>
+      <c r="H83" s="24"/>
+      <c r="I83" s="24"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B84" s="1" t="str" cm="1">
+        <f t="array" ref="B84">INDEX($B$8:$I$31,INT((ROW(B84)-49)/2)+1,COLUMN(B84)-1)</f>
         <v>Mode choice</v>
       </c>
-      <c r="C81" s="2" t="str" cm="1">
-        <f t="array" ref="C81">INDEX($B$8:$I$30,INT((ROW(C81)-49)/2)+1,COLUMN(C81)-1)</f>
+      <c r="C84" s="1" t="str" cm="1">
+        <f t="array" ref="C84">INDEX($B$8:$I$31,INT((ROW(C84)-49)/2)+1,COLUMN(C84)-1)</f>
         <v>Mode choice</v>
       </c>
-      <c r="D81" s="2" t="str" cm="1">
-        <f t="array" ref="D81">INDEX($B$8:$I$30,INT((ROW(D81)-49)/2)+1,COLUMN(D81)-1)</f>
+      <c r="D84" s="1" t="str" cm="1">
+        <f t="array" ref="D84">INDEX($B$8:$I$31,INT((ROW(D84)-49)/2)+1,COLUMN(D84)-1)</f>
         <v>constant</v>
       </c>
-      <c r="E81" s="2" t="str" cm="1">
-        <f t="array" ref="E81">INDEX($B$8:$I$30,INT((ROW(E81)-49)/2)+1,COLUMN(E81)-1)</f>
+      <c r="E84" s="1" t="str" cm="1">
+        <f t="array" ref="E84">INDEX($B$8:$I$31,INT((ROW(E84)-49)/2)+1,COLUMN(E84)-1)</f>
         <v>PERCEPTION TIME</v>
       </c>
-      <c r="F81" s="2" cm="1">
-        <f t="array" ref="F81">INDEX($B$8:$I$30,INT((ROW(F81)-49)/2)+1,COLUMN(F81)-1)</f>
+      <c r="F84" s="1" cm="1">
+        <f t="array" ref="F84">INDEX($B$8:$I$31,INT((ROW(F84)-49)/2)+1,COLUMN(F84)-1)</f>
         <v>1</v>
       </c>
-      <c r="G81" s="2" cm="1">
-        <f t="array" ref="G81">INDEX($B$8:$I$30,INT((ROW(G81)-49)/2)+1,COLUMN(G81)-1)</f>
+      <c r="G84" s="1" cm="1">
+        <f t="array" ref="G84">INDEX($B$8:$I$31,INT((ROW(G84)-49)/2)+1,COLUMN(G84)-1)</f>
         <v>5</v>
       </c>
-      <c r="H81" s="2" cm="1">
-        <f t="array" ref="H81">INDEX($B$8:$I$30,INT((ROW(H81)-49)/2)+1,COLUMN(H81)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I81" s="2" t="str" cm="1">
-        <f t="array" ref="I81">INDEX($B$8:$I$30,INT((ROW(I81)-49)/2)+1,COLUMN(I81)-1)</f>
+      <c r="H84" s="1" cm="1">
+        <f t="array" ref="H84">INDEX($B$8:$I$31,INT((ROW(H84)-49)/2)+1,COLUMN(H84)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I84" s="1" t="str" cm="1">
+        <f t="array" ref="I84">INDEX($B$8:$I$31,INT((ROW(I84)-49)/2)+1,COLUMN(I84)-1)</f>
         <v>Year</v>
       </c>
     </row>
-    <row r="82" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B82" s="3" t="str" cm="1">
-        <f t="array" ref="B82">IF(MOD(ROW(B82)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B82)-49)/2)+1),"")</f>
+    <row r="85" spans="2:9" ht="43.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B85" s="24" t="str" cm="1">
+        <f t="array" ref="B85">IF(MOD(ROW(B84)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B84)-49)/2)+1),"")</f>
         <v>Perception time determines how fast travel behavior adapts to changes in relative attractiveness, by setting a delay to changes in perceived attractiveness of modes resulting from changes in subjective travel time. A wide range is taken between 1 and 5 years.</v>
       </c>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="3"/>
-      <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
-    </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B83" s="2" t="str" cm="1">
-        <f t="array" ref="B83">INDEX($B$8:$I$30,INT((ROW(B83)-49)/2)+1,COLUMN(B83)-1)</f>
+      <c r="C85" s="24"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="24"/>
+      <c r="H85" s="24"/>
+      <c r="I85" s="24"/>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B86" s="1" t="str" cm="1">
+        <f t="array" ref="B86">INDEX($B$8:$I$31,INT((ROW(B86)-49)/2)+1,COLUMN(B86)-1)</f>
         <v>Mode choice</v>
       </c>
-      <c r="C83" s="2" t="str" cm="1">
-        <f t="array" ref="C83">INDEX($B$8:$I$30,INT((ROW(C83)-49)/2)+1,COLUMN(C83)-1)</f>
+      <c r="C86" s="1" t="str" cm="1">
+        <f t="array" ref="C86">INDEX($B$8:$I$31,INT((ROW(C86)-49)/2)+1,COLUMN(C86)-1)</f>
         <v>Data</v>
       </c>
-      <c r="D83" s="2" t="str" cm="1">
-        <f t="array" ref="D83">INDEX($B$8:$I$30,INT((ROW(D83)-49)/2)+1,COLUMN(D83)-1)</f>
+      <c r="D86" s="1" t="str" cm="1">
+        <f t="array" ref="D86">INDEX($B$8:$I$31,INT((ROW(D86)-49)/2)+1,COLUMN(D86)-1)</f>
         <v>effect sensitivity</v>
       </c>
-      <c r="E83" s="2" t="str" cm="1">
-        <f t="array" ref="E83">INDEX($B$8:$I$30,INT((ROW(E83)-49)/2)+1,COLUMN(E83)-1)</f>
+      <c r="E86" s="1" t="str" cm="1">
+        <f t="array" ref="E86">INDEX($B$8:$I$31,INT((ROW(E86)-49)/2)+1,COLUMN(E86)-1)</f>
         <v>SENSITIVITY TO SIDEWALK DATA UNCERTAINTY</v>
       </c>
-      <c r="F83" s="2" cm="1">
-        <f t="array" ref="F83">INDEX($B$8:$I$30,INT((ROW(F83)-49)/2)+1,COLUMN(F83)-1)</f>
+      <c r="F86" s="1" cm="1">
+        <f t="array" ref="F86">INDEX($B$8:$I$31,INT((ROW(F86)-49)/2)+1,COLUMN(F86)-1)</f>
         <v>0.5</v>
       </c>
-      <c r="G83" s="2" cm="1">
-        <f t="array" ref="G83">INDEX($B$8:$I$30,INT((ROW(G83)-49)/2)+1,COLUMN(G83)-1)</f>
+      <c r="G86" s="1" cm="1">
+        <f t="array" ref="G86">INDEX($B$8:$I$31,INT((ROW(G86)-49)/2)+1,COLUMN(G86)-1)</f>
         <v>2</v>
       </c>
-      <c r="H83" s="2" cm="1">
-        <f t="array" ref="H83">INDEX($B$8:$I$30,INT((ROW(H83)-49)/2)+1,COLUMN(H83)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I83" s="2" t="str" cm="1">
-        <f t="array" ref="I83">INDEX($B$8:$I$30,INT((ROW(I83)-49)/2)+1,COLUMN(I83)-1)</f>
+      <c r="H86" s="1" cm="1">
+        <f t="array" ref="H86">INDEX($B$8:$I$31,INT((ROW(H86)-49)/2)+1,COLUMN(H86)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I86" s="1" t="str" cm="1">
+        <f t="array" ref="I86">INDEX($B$8:$I$31,INT((ROW(I86)-49)/2)+1,COLUMN(I86)-1)</f>
         <v>Dmnl</v>
       </c>
     </row>
-    <row r="84" spans="2:9" ht="43.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B84" s="3" t="str" cm="1">
-        <f t="array" ref="B84">IF(MOD(ROW(B84)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B84)-49)/2)+1),"")</f>
+    <row r="87" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B87" s="24" t="str" cm="1">
+        <f t="array" ref="B87">IF(MOD(ROW(B86)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B86)-49)/2)+1),"")</f>
         <v>The base assumption is for PT access egress time to increase by 400% if no sidewalks existed, and to halve when pedestrian space were to double (see Appendix ). Since this effect size is uncertain, and because there is uncertainty in the estimated share of pedestrian space due to data gaps, the effect is varied by X^y if X is the normalized effect from the base assumption, and y varies between 0.5 and 2.</v>
       </c>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="3"/>
-      <c r="H84" s="3"/>
-      <c r="I84" s="3"/>
-    </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B85" s="2" t="str" cm="1">
-        <f t="array" ref="B85">INDEX($B$8:$I$30,INT((ROW(B85)-49)/2)+1,COLUMN(B85)-1)</f>
+      <c r="C87" s="24"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="24"/>
+      <c r="H87" s="24"/>
+      <c r="I87" s="24"/>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B88" s="1" t="str" cm="1">
+        <f t="array" ref="B88">INDEX($B$8:$I$31,INT((ROW(B88)-49)/2)+1,COLUMN(B88)-1)</f>
         <v>Mode choice</v>
       </c>
-      <c r="C85" s="2" t="str" cm="1">
-        <f t="array" ref="C85">INDEX($B$8:$I$30,INT((ROW(C85)-49)/2)+1,COLUMN(C85)-1)</f>
+      <c r="C88" s="1" t="str" cm="1">
+        <f t="array" ref="C88">INDEX($B$8:$I$31,INT((ROW(C88)-49)/2)+1,COLUMN(C88)-1)</f>
         <v>Data</v>
       </c>
-      <c r="D85" s="2" t="str" cm="1">
-        <f t="array" ref="D85">INDEX($B$8:$I$30,INT((ROW(D85)-49)/2)+1,COLUMN(D85)-1)</f>
+      <c r="D88" s="1" t="str" cm="1">
+        <f t="array" ref="D88">INDEX($B$8:$I$31,INT((ROW(D88)-49)/2)+1,COLUMN(D88)-1)</f>
         <v>effect sensitivity</v>
       </c>
-      <c r="E85" s="2" t="str" cm="1">
-        <f t="array" ref="E85">INDEX($B$8:$I$30,INT((ROW(E85)-49)/2)+1,COLUMN(E85)-1)</f>
+      <c r="E88" s="1" t="str" cm="1">
+        <f t="array" ref="E88">INDEX($B$8:$I$31,INT((ROW(E88)-49)/2)+1,COLUMN(E88)-1)</f>
         <v>SENSITIVITY TO CAR LANE DATA UNCERTAINTY</v>
       </c>
-      <c r="F85" s="2" cm="1">
-        <f t="array" ref="F85">INDEX($B$8:$I$30,INT((ROW(F85)-49)/2)+1,COLUMN(F85)-1)</f>
+      <c r="F88" s="1" cm="1">
+        <f t="array" ref="F88">INDEX($B$8:$I$31,INT((ROW(F88)-49)/2)+1,COLUMN(F88)-1)</f>
         <v>0.5</v>
       </c>
-      <c r="G85" s="2" cm="1">
-        <f t="array" ref="G85">INDEX($B$8:$I$30,INT((ROW(G85)-49)/2)+1,COLUMN(G85)-1)</f>
+      <c r="G88" s="1" cm="1">
+        <f t="array" ref="G88">INDEX($B$8:$I$31,INT((ROW(G88)-49)/2)+1,COLUMN(G88)-1)</f>
         <v>2</v>
       </c>
-      <c r="H85" s="2" cm="1">
-        <f t="array" ref="H85">INDEX($B$8:$I$30,INT((ROW(H85)-49)/2)+1,COLUMN(H85)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I85" s="2" t="str" cm="1">
-        <f t="array" ref="I85">INDEX($B$8:$I$30,INT((ROW(I85)-49)/2)+1,COLUMN(I85)-1)</f>
+      <c r="H88" s="1" cm="1">
+        <f t="array" ref="H88">INDEX($B$8:$I$31,INT((ROW(H88)-49)/2)+1,COLUMN(H88)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I88" s="1" t="str" cm="1">
+        <f t="array" ref="I88">INDEX($B$8:$I$31,INT((ROW(I88)-49)/2)+1,COLUMN(I88)-1)</f>
         <v>Dmnl</v>
       </c>
     </row>
-    <row r="86" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B86" s="3" t="str" cm="1">
-        <f t="array" ref="B86">IF(MOD(ROW(B86)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B86)-49)/2)+1),"")</f>
+    <row r="89" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B89" s="24" t="str" cm="1">
+        <f t="array" ref="B89">IF(MOD(ROW(B88)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B88)-49)/2)+1),"")</f>
         <v>The base assumption is for subjective cost factor of cycling time to fall by 0.1 or increase by 0.2 Minutes/Minute depending on whether theaverage road is oneway or four-lane (see Appendix ). Since this effect size is uncertain, and because there is uncertainty in the estimated share of road space due to data gaps, the effect is varied by X^y if X is the normalized effect from the base assumption, and y varies between 0.5 and 2.</v>
       </c>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
-      <c r="G86" s="3"/>
-      <c r="H86" s="3"/>
-      <c r="I86" s="3"/>
-    </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B87" s="2" t="str" cm="1">
-        <f t="array" ref="B87">INDEX($B$8:$I$30,INT((ROW(B87)-49)/2)+1,COLUMN(B87)-1)</f>
+      <c r="C89" s="24"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="24"/>
+      <c r="H89" s="24"/>
+      <c r="I89" s="24"/>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B90" s="1" t="str" cm="1">
+        <f t="array" ref="B90">INDEX($B$8:$I$31,INT((ROW(B90)-49)/2)+1,COLUMN(B90)-1)</f>
         <v>Mode choice</v>
       </c>
-      <c r="C87" s="2" t="str" cm="1">
-        <f t="array" ref="C87">INDEX($B$8:$I$30,INT((ROW(C87)-49)/2)+1,COLUMN(C87)-1)</f>
+      <c r="C90" s="1" t="str" cm="1">
+        <f t="array" ref="C90">INDEX($B$8:$I$31,INT((ROW(C90)-49)/2)+1,COLUMN(C90)-1)</f>
         <v>Future policy</v>
       </c>
-      <c r="D87" s="2" t="str" cm="1">
-        <f t="array" ref="D87">INDEX($B$8:$I$30,INT((ROW(D87)-49)/2)+1,COLUMN(D87)-1)</f>
+      <c r="D90" s="1" t="str" cm="1">
+        <f t="array" ref="D90">INDEX($B$8:$I$31,INT((ROW(D90)-49)/2)+1,COLUMN(D90)-1)</f>
         <v>constant</v>
       </c>
-      <c r="E87" s="2" t="str" cm="1">
-        <f t="array" ref="E87">INDEX($B$8:$I$30,INT((ROW(E87)-49)/2)+1,COLUMN(E87)-1)</f>
+      <c r="E90" s="1" t="str" cm="1">
+        <f t="array" ref="E90">INDEX($B$8:$I$31,INT((ROW(E90)-49)/2)+1,COLUMN(E90)-1)</f>
         <v>NET ADDED PT CAPACITY PER YEAR</v>
       </c>
-      <c r="F87" s="2" cm="1">
-        <f t="array" ref="F87">INDEX($B$8:$I$30,INT((ROW(F87)-49)/2)+1,COLUMN(F87)-1)</f>
+      <c r="F90" s="1" cm="1">
+        <f t="array" ref="F90">INDEX($B$8:$I$31,INT((ROW(F90)-49)/2)+1,COLUMN(F90)-1)</f>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G87" s="2" cm="1">
-        <f t="array" ref="G87">INDEX($B$8:$I$30,INT((ROW(G87)-49)/2)+1,COLUMN(G87)-1)</f>
+      <c r="G90" s="1" cm="1">
+        <f t="array" ref="G90">INDEX($B$8:$I$31,INT((ROW(G90)-49)/2)+1,COLUMN(G90)-1)</f>
         <v>1.5E-3</v>
       </c>
-      <c r="H87" s="2" cm="1">
-        <f t="array" ref="H87">INDEX($B$8:$I$30,INT((ROW(H87)-49)/2)+1,COLUMN(H87)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I87" s="2" t="str" cm="1">
-        <f t="array" ref="I87">INDEX($B$8:$I$30,INT((ROW(I87)-49)/2)+1,COLUMN(I87)-1)</f>
+      <c r="H90" s="1" cm="1">
+        <f t="array" ref="H90">INDEX($B$8:$I$31,INT((ROW(H90)-49)/2)+1,COLUMN(H90)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I90" s="1" t="str" cm="1">
+        <f t="array" ref="I90">INDEX($B$8:$I$31,INT((ROW(I90)-49)/2)+1,COLUMN(I90)-1)</f>
         <v>Dmnl/Year</v>
       </c>
     </row>
-    <row r="88" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B88" s="3" t="str" cm="1">
-        <f t="array" ref="B88">IF(MOD(ROW(B88)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B88)-49)/2)+1),"")</f>
+    <row r="91" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B91" s="24" t="str" cm="1">
+        <f t="array" ref="B91">IF(MOD(ROW(B90)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B90)-49)/2)+1),"")</f>
         <v>The metro system is being expanded and automation increases the frequency and thus capacity of the metro system. Given the size of the metro system, and the pace of public transport infrastructure construction being in the order of decades, an order of magnitude of 1% per decade is plausible. Due to uncertainty, the variable is varied between 0.5% and 1.5% per decade</v>
       </c>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
-      <c r="G88" s="3"/>
-      <c r="H88" s="3"/>
-      <c r="I88" s="3"/>
-    </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B89" s="2" t="str" cm="1">
-        <f t="array" ref="B89">INDEX($B$8:$I$30,INT((ROW(B89)-49)/2)+1,COLUMN(B89)-1)</f>
+      <c r="C91" s="24"/>
+      <c r="D91" s="24"/>
+      <c r="E91" s="24"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="24"/>
+      <c r="H91" s="24"/>
+      <c r="I91" s="24"/>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B92" s="1" t="str" cm="1">
+        <f t="array" ref="B92">INDEX($B$8:$I$31,INT((ROW(B92)-49)/2)+1,COLUMN(B92)-1)</f>
         <v>Destination choice</v>
       </c>
-      <c r="C89" s="2" t="str" cm="1">
-        <f t="array" ref="C89">INDEX($B$8:$I$30,INT((ROW(C89)-49)/2)+1,COLUMN(C89)-1)</f>
+      <c r="C92" s="1" t="str" cm="1">
+        <f t="array" ref="C92">INDEX($B$8:$I$31,INT((ROW(C92)-49)/2)+1,COLUMN(C92)-1)</f>
         <v>Future policy, Destination choice</v>
       </c>
-      <c r="D89" s="2" t="str" cm="1">
-        <f t="array" ref="D89">INDEX($B$8:$I$30,INT((ROW(D89)-49)/2)+1,COLUMN(D89)-1)</f>
+      <c r="D92" s="1" t="str" cm="1">
+        <f t="array" ref="D92">INDEX($B$8:$I$31,INT((ROW(D92)-49)/2)+1,COLUMN(D92)-1)</f>
         <v>constant</v>
       </c>
-      <c r="E89" s="2" t="str" cm="1">
-        <f t="array" ref="E89">INDEX($B$8:$I$30,INT((ROW(E89)-49)/2)+1,COLUMN(E89)-1)</f>
+      <c r="E92" s="1" t="str" cm="1">
+        <f t="array" ref="E92">INDEX($B$8:$I$31,INT((ROW(E92)-49)/2)+1,COLUMN(E92)-1)</f>
         <v>DESTINATION SHIFT RATE RING</v>
       </c>
-      <c r="F89" s="2" cm="1">
-        <f t="array" ref="F89">INDEX($B$8:$I$30,INT((ROW(F89)-49)/2)+1,COLUMN(F89)-1)</f>
+      <c r="F92" s="1" cm="1">
+        <f t="array" ref="F92">INDEX($B$8:$I$31,INT((ROW(F92)-49)/2)+1,COLUMN(F92)-1)</f>
         <v>1E-3</v>
       </c>
-      <c r="G89" s="2" cm="1">
-        <f t="array" ref="G89">INDEX($B$8:$I$30,INT((ROW(G89)-49)/2)+1,COLUMN(G89)-1)</f>
+      <c r="G92" s="1" cm="1">
+        <f t="array" ref="G92">INDEX($B$8:$I$31,INT((ROW(G92)-49)/2)+1,COLUMN(G92)-1)</f>
         <v>0.01</v>
       </c>
-      <c r="H89" s="2" cm="1">
-        <f t="array" ref="H89">INDEX($B$8:$I$30,INT((ROW(H89)-49)/2)+1,COLUMN(H89)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I89" s="2" t="str" cm="1">
-        <f t="array" ref="I89">INDEX($B$8:$I$30,INT((ROW(I89)-49)/2)+1,COLUMN(I89)-1)</f>
+      <c r="H92" s="1" cm="1">
+        <f t="array" ref="H92">INDEX($B$8:$I$31,INT((ROW(H92)-49)/2)+1,COLUMN(H92)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I92" s="1" t="str" cm="1">
+        <f t="array" ref="I92">INDEX($B$8:$I$31,INT((ROW(I92)-49)/2)+1,COLUMN(I92)-1)</f>
         <v>Dmnl/Year</v>
       </c>
     </row>
-    <row r="90" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B90" s="3" t="str" cm="1">
-        <f t="array" ref="B90">IF(MOD(ROW(B90)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B90)-49)/2)+1),"")</f>
+    <row r="93" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B93" s="24" t="str" cm="1">
+        <f t="array" ref="B93">IF(MOD(ROW(B92)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B92)-49)/2)+1),"")</f>
         <v>Destination choice is expected to change such that people travel less to the city, but it is uncertain to what extent. Change rates between 1% and 10% per decade are plausible, although further research is needed to refine this assumption</v>
       </c>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
-      <c r="E90" s="3"/>
-      <c r="F90" s="3"/>
-      <c r="G90" s="3"/>
-      <c r="H90" s="3"/>
-      <c r="I90" s="3"/>
-    </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B91" s="2" t="str" cm="1">
-        <f t="array" ref="B91">INDEX($B$8:$I$30,INT((ROW(B91)-49)/2)+1,COLUMN(B91)-1)</f>
+      <c r="C93" s="24"/>
+      <c r="D93" s="24"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="24"/>
+      <c r="G93" s="24"/>
+      <c r="H93" s="24"/>
+      <c r="I93" s="24"/>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B94" s="1" t="str" cm="1">
+        <f t="array" ref="B94">INDEX($B$8:$I$31,INT((ROW(B94)-49)/2)+1,COLUMN(B94)-1)</f>
         <v>Destination choice</v>
       </c>
-      <c r="C91" s="2" t="str" cm="1">
-        <f t="array" ref="C91">INDEX($B$8:$I$30,INT((ROW(C91)-49)/2)+1,COLUMN(C91)-1)</f>
+      <c r="C94" s="1" t="str" cm="1">
+        <f t="array" ref="C94">INDEX($B$8:$I$31,INT((ROW(C94)-49)/2)+1,COLUMN(C94)-1)</f>
         <v>Future policy, Destination choice</v>
       </c>
-      <c r="D91" s="2" t="str" cm="1">
-        <f t="array" ref="D91">INDEX($B$8:$I$30,INT((ROW(D91)-49)/2)+1,COLUMN(D91)-1)</f>
+      <c r="D94" s="1" t="str" cm="1">
+        <f t="array" ref="D94">INDEX($B$8:$I$31,INT((ROW(D94)-49)/2)+1,COLUMN(D94)-1)</f>
         <v>constant</v>
       </c>
-      <c r="E91" s="2" t="str" cm="1">
-        <f t="array" ref="E91">INDEX($B$8:$I$30,INT((ROW(E91)-49)/2)+1,COLUMN(E91)-1)</f>
+      <c r="E94" s="1" t="str" cm="1">
+        <f t="array" ref="E94">INDEX($B$8:$I$31,INT((ROW(E94)-49)/2)+1,COLUMN(E94)-1)</f>
         <v>DESTINATION SHIFT RATE CITY</v>
       </c>
-      <c r="F91" s="2" cm="1">
-        <f t="array" ref="F91">INDEX($B$8:$I$30,INT((ROW(F91)-49)/2)+1,COLUMN(F91)-1)</f>
+      <c r="F94" s="1" cm="1">
+        <f t="array" ref="F94">INDEX($B$8:$I$31,INT((ROW(F94)-49)/2)+1,COLUMN(F94)-1)</f>
         <v>1E-3</v>
       </c>
-      <c r="G91" s="2" cm="1">
-        <f t="array" ref="G91">INDEX($B$8:$I$30,INT((ROW(G91)-49)/2)+1,COLUMN(G91)-1)</f>
+      <c r="G94" s="1" cm="1">
+        <f t="array" ref="G94">INDEX($B$8:$I$31,INT((ROW(G94)-49)/2)+1,COLUMN(G94)-1)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H91" s="2" cm="1">
-        <f t="array" ref="H91">INDEX($B$8:$I$30,INT((ROW(H91)-49)/2)+1,COLUMN(H91)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="I91" s="2" t="str" cm="1">
-        <f t="array" ref="I91">INDEX($B$8:$I$30,INT((ROW(I91)-49)/2)+1,COLUMN(I91)-1)</f>
+      <c r="H94" s="1" cm="1">
+        <f t="array" ref="H94">INDEX($B$8:$I$31,INT((ROW(H94)-49)/2)+1,COLUMN(H94)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="I94" s="1" t="str" cm="1">
+        <f t="array" ref="I94">INDEX($B$8:$I$31,INT((ROW(I94)-49)/2)+1,COLUMN(I94)-1)</f>
         <v>Dmnl/Year</v>
       </c>
     </row>
-    <row r="92" spans="2:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B92" s="1" t="str" cm="1">
-        <f t="array" ref="B92">IF(MOD(ROW(B92)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B92)-49)/2)+1),"")</f>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B95" s="24" t="str" cm="1">
+        <f t="array" ref="B95">IF(MOD(ROW(B94)-49,2)=1,INDEX($J$8:$J$30,INT((ROW(B94)-49)/2)+1),"")</f>
         <v>Destination choice is expected to change such that people travel shorter distances within the city, but it is uncertain to what extent. Change rates between 1% and 5% per decade are plausible, although further research is needed to refine this assumption</v>
       </c>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
-      <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
-      <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
-      <c r="I92" s="1"/>
+      <c r="C95" s="24"/>
+      <c r="D95" s="24"/>
+      <c r="E95" s="24"/>
+      <c r="F95" s="24"/>
+      <c r="G95" s="24"/>
+      <c r="H95" s="24"/>
+      <c r="I95" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="B82:I82"/>
-    <mergeCell ref="B84:I84"/>
-    <mergeCell ref="B88:I88"/>
-    <mergeCell ref="B66:I66"/>
-    <mergeCell ref="B68:I68"/>
-    <mergeCell ref="B70:I70"/>
-    <mergeCell ref="B72:I72"/>
-    <mergeCell ref="B74:I74"/>
-    <mergeCell ref="B86:I86"/>
-    <mergeCell ref="B76:I76"/>
-    <mergeCell ref="B78:I78"/>
-    <mergeCell ref="B80:I80"/>
-    <mergeCell ref="B92:I92"/>
-    <mergeCell ref="B90:I90"/>
-    <mergeCell ref="B50:I50"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B54:I54"/>
-    <mergeCell ref="B56:I56"/>
-    <mergeCell ref="B58:I58"/>
-    <mergeCell ref="B60:I60"/>
-    <mergeCell ref="B62:I62"/>
-    <mergeCell ref="B64:I64"/>
+  <mergeCells count="23">
+    <mergeCell ref="B95:I95"/>
+    <mergeCell ref="B73:I73"/>
+    <mergeCell ref="B75:I75"/>
+    <mergeCell ref="B87:I87"/>
+    <mergeCell ref="B77:I77"/>
+    <mergeCell ref="B79:I79"/>
+    <mergeCell ref="B81:I81"/>
+    <mergeCell ref="B93:I93"/>
+    <mergeCell ref="B91:I91"/>
+    <mergeCell ref="B51:I51"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="B55:I55"/>
+    <mergeCell ref="B57:I57"/>
+    <mergeCell ref="B59:I59"/>
+    <mergeCell ref="B61:I61"/>
+    <mergeCell ref="B63:I63"/>
+    <mergeCell ref="B65:I65"/>
+    <mergeCell ref="B83:I83"/>
+    <mergeCell ref="B85:I85"/>
+    <mergeCell ref="B89:I89"/>
+    <mergeCell ref="B67:I67"/>
+    <mergeCell ref="B69:I69"/>
+    <mergeCell ref="B71:I71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>